<commit_message>
Upload current progress (see detailed message), development is pause for now...
</commit_message>
<xml_diff>
--- a/hardware/etc/TPS55288 Design Calculation V1.0.xlsx
+++ b/hardware/etc/TPS55288 Design Calculation V1.0.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Projects\StaticElecWand\hardware\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Projects\eWand\hardware\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552E9AC9-A723-4004-85D4-01679F755FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAE62C3-28C7-4F4C-97C4-A8D84A7F9062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="E023" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Calculation" sheetId="1" r:id="rId1"/>
@@ -88,10 +88,22 @@
     <definedName name="Vout_LP">'Design Calculation'!$C$73</definedName>
     <definedName name="Vout_max">'Design Calculation'!$C$18</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="TI User - Personal View" guid="{0F8159A6-236F-4F54-A569-A835A6AD5DA8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="803" activeSheetId="1"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1285,13 +1297,13 @@
     <t>TI Information - Selective Disclosure. You may not use the Program in non-TI devices.</t>
   </si>
   <si>
-    <t>ON -1</t>
-  </si>
-  <si>
     <t>EXT -1</t>
   </si>
   <si>
     <t>INT -1</t>
+  </si>
+  <si>
+    <t>OFF -0</t>
   </si>
 </sst>
 </file>
@@ -2697,127 +2709,127 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>25.464769014426569</c:v>
+                  <c:v>22.133569938468</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.131355468926941</c:v>
+                  <c:v>20.12132113588536</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.708910431112834</c:v>
+                  <c:v>18.103889199920886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.215482641999262</c:v>
+                  <c:v>16.081148374233841</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.689918627452</c:v>
+                  <c:v>14.054147983648374</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.18189169063429</c:v>
+                  <c:v>12.025381853602887</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.735096614450665</c:v>
+                  <c:v>9.9983050379573584</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.3743063884077866</c:v>
+                  <c:v>7.976288849245539</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1032819782090266</c:v>
+                  <c:v>5.9618232287959367</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9113851681655283</c:v>
+                  <c:v>3.9565573093388839</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7822641088583582</c:v>
+                  <c:v>1.9620431431125827</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.29991251500629795</c:v>
+                  <c:v>-1.9264260001200916E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.3474724188215106</c:v>
+                  <c:v>-1.9829924314828746</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-4.3684099841019499</c:v>
+                  <c:v>-3.9218062873989981</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-6.3664599866553919</c:v>
+                  <c:v>-5.8242683806764175</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-8.3412930852878446</c:v>
+                  <c:v>-7.6737260907647027</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-10.288511251654851</c:v>
+                  <c:v>-9.447766167656015</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-12.199471899301136</c:v>
+                  <c:v>-11.11938722802323</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-14.06130847811572</c:v>
+                  <c:v>-12.661455077775946</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-15.857891261151529</c:v>
+                  <c:v>-14.055195579160827</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-17.572645285029381</c:v>
+                  <c:v>-15.30045758302904</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-19.193432416818641</c:v>
+                  <c:v>-16.421632928543687</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-20.717633028097545</c:v>
+                  <c:v>-17.46310195417762</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-22.153728212699104</c:v>
+                  <c:v>-18.474625557705252</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-23.517783084198314</c:v>
+                  <c:v>-19.495485102541128</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-24.82910957535637</c:v>
+                  <c:v>-20.548293079954504</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-26.111291514630874</c:v>
+                  <c:v>-21.646368818765854</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-27.397850629390796</c:v>
+                  <c:v>-22.807546525289084</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-28.734211676491931</c:v>
+                  <c:v>-24.0618761752281</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-30.170205396250175</c:v>
+                  <c:v>-25.446786954126146</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-31.747938453419621</c:v>
+                  <c:v>-26.995557844965123</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-33.495414619638382</c:v>
+                  <c:v>-28.730572074459772</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-35.430672149749014</c:v>
+                  <c:v>-30.666753119211613</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-37.572291492263162</c:v>
+                  <c:v>-32.821241474069758</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-39.948984012561297</c:v>
+                  <c:v>-35.221990791410718</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-42.603393235039213</c:v>
+                  <c:v>-37.910408764242867</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-45.588938953326902</c:v>
+                  <c:v>-40.937197820975626</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-48.961933666525013</c:v>
+                  <c:v>-44.354310655463209</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-52.773633821396245</c:v>
+                  <c:v>-48.208076849190903</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-57.065796262774811</c:v>
+                  <c:v>-52.536411056416839</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-61.868542300159561</c:v>
+                  <c:v>-57.367667784208621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2991,127 +3003,127 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>79.41194383824508</c:v>
+                  <c:v>89.902840009363658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.304433100763788</c:v>
+                  <c:v>89.301243024768041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.50226070658411</c:v>
+                  <c:v>88.697199908309685</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.233380830043899</c:v>
+                  <c:v>88.077224083059889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73.654430925619607</c:v>
+                  <c:v>87.428541595236481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.767428579704003</c:v>
+                  <c:v>86.731958089671579</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.405261052728335</c:v>
+                  <c:v>85.954195833808654</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.296588350902027</c:v>
+                  <c:v>85.044426714829086</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76.158990956845713</c:v>
+                  <c:v>83.936437980198946</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76.762075478306571</c:v>
+                  <c:v>82.552699184412077</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>76.942527937914832</c:v>
+                  <c:v>80.806018988045665</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>76.587595286264232</c:v>
+                  <c:v>78.597897756451772</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>75.609250528980056</c:v>
+                  <c:v>75.815420634979802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73.921777727361587</c:v>
+                  <c:v>72.329234826084132</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71.426570438845516</c:v>
+                  <c:v>67.995247519860527</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68.004227403844425</c:v>
+                  <c:v>62.663179335932995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>63.514108772929895</c:v>
+                  <c:v>56.195573365116211</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>57.803289866702855</c:v>
+                  <c:v>48.499413403491999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50.728699893184221</c:v>
+                  <c:v>39.566400291006516</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42.19598899006327</c:v>
+                  <c:v>29.506885500519584</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.212700305562194</c:v>
+                  <c:v>18.554748756933943</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20.938676054605764</c:v>
+                  <c:v>7.0303727536125749</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.6988270762513338</c:v>
+                  <c:v>-4.7261195654965888</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-4.0771874159060104</c:v>
+                  <c:v>-16.42771940852813</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-16.987823622718309</c:v>
+                  <c:v>-27.908779786806925</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-29.80804922765746</c:v>
+                  <c:v>-39.182081442155734</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-42.569881100255273</c:v>
+                  <c:v>-50.457823532128614</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-55.527929862906134</c:v>
+                  <c:v>-62.093962396478432</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-69.041023330989319</c:v>
+                  <c:v>-74.492264502207533</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-83.46084216117076</c:v>
+                  <c:v>-88.009268518982125</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-99.104320943424469</c:v>
+                  <c:v>-102.94684863423294</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-116.30910318214974</c:v>
+                  <c:v>-119.61863620667266</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-135.50938020374556</c:v>
+                  <c:v>-138.43071408227925</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-157.27549358081262</c:v>
+                  <c:v>-159.92208236113217</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-182.30570384895836</c:v>
+                  <c:v>-184.75574350522641</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-211.39237903675581</c:v>
+                  <c:v>-213.68567191529041</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-244.65802222475335</c:v>
+                  <c:v>-246.79787806573549</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-261.0234648153745</c:v>
+                  <c:v>-262.98749116169006</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-278.23994847241528</c:v>
+                  <c:v>-279.99794010202032</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-296.03918560911262</c:v>
+                  <c:v>-297.56998901036326</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-314.07186125076487</c:v>
+                  <c:v>-315.37168354301792</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3335,8 +3347,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6930934" y="13607144"/>
-          <a:ext cx="6905897" cy="5290456"/>
+          <a:off x="7057934" y="13047074"/>
+          <a:ext cx="7036707" cy="5084716"/>
           <a:chOff x="6669810" y="12666539"/>
           <a:chExt cx="6585857" cy="4008623"/>
         </a:xfrm>
@@ -3412,15 +3424,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>53340</xdr:colOff>
+          <xdr:colOff>50800</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>220980</xdr:colOff>
+          <xdr:colOff>222250</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3754,29 +3766,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45:P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="108" customWidth="1"/>
+    <col min="1" max="1" width="2.6328125" style="108" customWidth="1"/>
     <col min="2" max="2" width="24" style="61" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="61" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="61" customWidth="1"/>
-    <col min="5" max="5" width="53.88671875" style="61" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="61" customWidth="1"/>
-    <col min="7" max="11" width="8.88671875" style="61" customWidth="1"/>
-    <col min="12" max="13" width="8.88671875" style="61"/>
-    <col min="14" max="14" width="13.109375" style="61" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.88671875" style="61"/>
-    <col min="17" max="17" width="2.6640625" style="61" customWidth="1"/>
-    <col min="18" max="19" width="8.88671875" style="61"/>
-    <col min="20" max="20" width="8.88671875" style="61" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="61"/>
+    <col min="3" max="3" width="13.36328125" style="61" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="61" customWidth="1"/>
+    <col min="5" max="5" width="53.90625" style="61" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" style="61" customWidth="1"/>
+    <col min="7" max="11" width="8.90625" style="61" customWidth="1"/>
+    <col min="12" max="13" width="8.90625" style="61"/>
+    <col min="14" max="14" width="13.08984375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.90625" style="61"/>
+    <col min="17" max="17" width="2.6328125" style="61" customWidth="1"/>
+    <col min="18" max="19" width="8.90625" style="61"/>
+    <col min="20" max="20" width="8.90625" style="61" customWidth="1"/>
+    <col min="21" max="16384" width="8.90625" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13.8" thickBot="1">
+    <row r="1" spans="1:17" ht="13" thickBot="1">
       <c r="A1" s="58"/>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -3795,7 +3807,7 @@
       <c r="P1" s="60"/>
       <c r="Q1" s="60"/>
     </row>
-    <row r="2" spans="1:17" ht="16.2" thickTop="1">
+    <row r="2" spans="1:17" ht="16" thickTop="1">
       <c r="A2" s="58"/>
       <c r="B2" s="140" t="s">
         <v>284</v>
@@ -3875,7 +3887,7 @@
       <c r="P5" s="65"/>
       <c r="Q5" s="60"/>
     </row>
-    <row r="6" spans="1:17" ht="13.2" customHeight="1">
+    <row r="6" spans="1:17" ht="13.25" customHeight="1">
       <c r="A6" s="58"/>
       <c r="B6" s="146" t="s">
         <v>39</v>
@@ -3915,7 +3927,7 @@
       <c r="P7" s="65"/>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="15.6">
+    <row r="8" spans="1:17" ht="15.5">
       <c r="A8" s="58"/>
       <c r="B8" s="66"/>
       <c r="C8" s="67"/>
@@ -3936,7 +3948,7 @@
       <c r="P8" s="65"/>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="15.6">
+    <row r="9" spans="1:17" ht="15.5">
       <c r="A9" s="58"/>
       <c r="B9" s="66"/>
       <c r="C9" s="70"/>
@@ -3957,7 +3969,7 @@
       <c r="P9" s="65"/>
       <c r="Q9" s="60"/>
     </row>
-    <row r="10" spans="1:17" ht="13.8">
+    <row r="10" spans="1:17" ht="14">
       <c r="A10" s="58"/>
       <c r="B10" s="66"/>
       <c r="C10" s="71"/>
@@ -3978,7 +3990,7 @@
       <c r="P10" s="65"/>
       <c r="Q10" s="60"/>
     </row>
-    <row r="11" spans="1:17" ht="13.8">
+    <row r="11" spans="1:17" ht="14">
       <c r="A11" s="58"/>
       <c r="B11" s="66"/>
       <c r="C11" s="64"/>
@@ -3997,7 +4009,7 @@
       <c r="P11" s="65"/>
       <c r="Q11" s="60"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" ht="13">
       <c r="A12" s="58"/>
       <c r="B12" s="72" t="s">
         <v>25</v>
@@ -4026,7 +4038,7 @@
       <c r="P12" s="150"/>
       <c r="Q12" s="60"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" ht="13">
       <c r="A13" s="58"/>
       <c r="B13" s="151" t="s">
         <v>43</v>
@@ -4187,7 +4199,7 @@
         <v>68</v>
       </c>
       <c r="C19" s="35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D19" s="78" t="s">
         <v>4</v>
@@ -4313,7 +4325,7 @@
       <c r="P23" s="65"/>
       <c r="Q23" s="60"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" ht="13">
       <c r="A24" s="58"/>
       <c r="B24" s="80" t="s">
         <v>60</v>
@@ -4341,7 +4353,7 @@
       <c r="P24" s="65"/>
       <c r="Q24" s="60"/>
     </row>
-    <row r="25" spans="1:17" ht="26.4">
+    <row r="25" spans="1:17" ht="25">
       <c r="A25" s="58"/>
       <c r="B25" s="77" t="s">
         <v>54</v>
@@ -4368,7 +4380,7 @@
       <c r="P25" s="65"/>
       <c r="Q25" s="60"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" ht="13">
       <c r="A26" s="58"/>
       <c r="B26" s="80" t="s">
         <v>55</v>
@@ -4427,7 +4439,7 @@
         <v>91</v>
       </c>
       <c r="C28" s="35">
-        <v>5</v>
+        <v>6.3</v>
       </c>
       <c r="D28" s="78" t="s">
         <v>4</v>
@@ -4475,14 +4487,14 @@
       <c r="P29" s="65"/>
       <c r="Q29" s="60"/>
     </row>
-    <row r="30" spans="1:17" ht="26.4">
+    <row r="30" spans="1:17" ht="25">
       <c r="A30" s="58"/>
       <c r="B30" s="77" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="41" t="str">
         <f>IF(Iout_limit*R_1&lt;=63.5,DEC2HEX(ROUNDUP(Iout_limit*R_1/0.5,0)+IF((C27="Enable"),128,0)),"error")</f>
-        <v>E4</v>
+        <v>FE</v>
       </c>
       <c r="D30" s="78" t="s">
         <v>52</v>
@@ -4503,14 +4515,14 @@
       <c r="P30" s="65"/>
       <c r="Q30" s="60"/>
     </row>
-    <row r="31" spans="1:17" ht="27">
+    <row r="31" spans="1:17" ht="25.5">
       <c r="A31" s="58"/>
       <c r="B31" s="77" t="s">
         <v>319</v>
       </c>
       <c r="C31" s="42">
         <f>IF((Vout&gt;Vin_min), SQRT((Vout-Vin_min)/Vin_min)*Ioutmax, 1/SQRT(12)*Vout*(1-Vout/Vin_max)/L/fsw)</f>
-        <v>5.196152422706632</v>
+        <v>8.6602540378443855</v>
       </c>
       <c r="D31" s="78" t="s">
         <v>19</v>
@@ -4531,14 +4543,14 @@
       <c r="P31" s="65"/>
       <c r="Q31" s="60"/>
     </row>
-    <row r="32" spans="1:17" ht="26.4">
+    <row r="32" spans="1:17" ht="25">
       <c r="A32" s="58"/>
       <c r="B32" s="77" t="s">
         <v>313</v>
       </c>
       <c r="C32" s="42">
         <f>IF((Vin_max&gt;Vout), IF(Vin_max&lt;(2*Vout), Ioutmax*SQRT(Vout*(Vin_max-Vout)/Vin_max/Vin_max), Ioutmax/2), IF(Vin_min&gt;Vout/2, 1/SQRT(12)*Vin_min*(1-Vin_min/Vout)/L/fsw, 1/SQRT(12)*Vout/4/L/fsw))</f>
-        <v>1.299038105676658</v>
+        <v>2.1650635094610964</v>
       </c>
       <c r="D32" s="78" t="s">
         <v>19</v>
@@ -4586,7 +4598,7 @@
       <c r="P33" s="65"/>
       <c r="Q33" s="60"/>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" ht="13">
       <c r="A34" s="58"/>
       <c r="B34" s="80" t="s">
         <v>36</v>
@@ -4641,7 +4653,7 @@
       <c r="P35" s="65"/>
       <c r="Q35" s="60"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" ht="13">
       <c r="A36" s="58"/>
       <c r="B36" s="80" t="s">
         <v>95</v>
@@ -4669,7 +4681,7 @@
       <c r="P36" s="154"/>
       <c r="Q36" s="60"/>
     </row>
-    <row r="37" spans="1:17" ht="27">
+    <row r="37" spans="1:17" ht="25.5">
       <c r="A37" s="58"/>
       <c r="B37" s="77" t="s">
         <v>320</v>
@@ -4703,7 +4715,7 @@
       </c>
       <c r="C38" s="47">
         <f>MAX((Vout-Vin_min)/Vout/fsw*Ioutmax/dVoutpkpk, 1/8/fsw*(ILpeak_max-ILvalley_max)/dVoutpkpk)</f>
-        <v>1.1396155696811609E-4</v>
+        <v>1.8993592828019348E-4</v>
       </c>
       <c r="D38" s="78" t="s">
         <v>9</v>
@@ -4972,7 +4984,7 @@
       </c>
       <c r="P43" s="124" t="str">
         <f>Reg_Ilimit</f>
-        <v>E4</v>
+        <v>FE</v>
       </c>
       <c r="Q43" s="60"/>
     </row>
@@ -4998,11 +5010,11 @@
       </c>
       <c r="K44" s="26" t="str">
         <f>MID(HEX2BIN(Reg_Ilimit, 8), 4, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" s="28" t="str">
         <f>MID(HEX2BIN(Reg_Ilimit, 8), 5, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" s="28" t="str">
         <f>MID(HEX2BIN(Reg_Ilimit, 8), 6, 1)</f>
@@ -5010,7 +5022,7 @@
       </c>
       <c r="N44" s="28" t="str">
         <f>MID(HEX2BIN(Reg_Ilimit, 8), 7, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" s="28" t="str">
         <f>MID(HEX2BIN(Reg_Ilimit, 8),8, 1)</f>
@@ -5065,7 +5077,7 @@
       </c>
       <c r="P45" s="124" t="str">
         <f>DEC2HEX((O46+N46*2+K46*16+J46*32),2)</f>
-        <v>01</v>
+        <v>31</v>
       </c>
       <c r="Q45" s="60"/>
     </row>
@@ -5085,11 +5097,11 @@
       </c>
       <c r="J46" s="28">
         <f>IF(OR((C66=0.1),(C66=3)),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" s="28">
         <f>IF(OR((C66=0.1),(C66=6)),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="87">
         <v>0</v>
@@ -5115,7 +5127,7 @@
       </c>
       <c r="C47" s="131">
         <f>Ioutmax*0.25/dVinpkpk/fsw</f>
-        <v>3.7987185656038693E-5</v>
+        <v>6.3311976093397831E-5</v>
       </c>
       <c r="D47" s="127" t="s">
         <v>9</v>
@@ -5333,7 +5345,7 @@
       </c>
       <c r="P51" s="124" t="str">
         <f>DEC2HEX(RIGHT(H52,1)*128+RIGHT(I52,1)*64+RIGHT(J52,1)*32+RIGHT(K52,1)*16+RIGHT(L52,1)*8+RIGHT(M52,1)*4+RIGHT(N52,1)*2+RIGHT(O52,1), 2)</f>
-        <v>B9</v>
+        <v>39</v>
       </c>
       <c r="Q51" s="60"/>
     </row>
@@ -5346,7 +5358,7 @@
       <c r="F52" s="113"/>
       <c r="G52" s="113"/>
       <c r="H52" s="22" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="I52" s="22" t="s">
         <v>237</v>
@@ -5358,7 +5370,7 @@
         <v>238</v>
       </c>
       <c r="L52" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M52" s="22" t="s">
         <v>239</v>
@@ -5367,7 +5379,7 @@
         <v>240</v>
       </c>
       <c r="O52" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P52" s="124"/>
       <c r="Q52" s="60"/>
@@ -5455,14 +5467,14 @@
       <c r="P54" s="115"/>
       <c r="Q54" s="60"/>
     </row>
-    <row r="55" spans="1:17" ht="26.4">
+    <row r="55" spans="1:17" ht="25">
       <c r="A55" s="58"/>
       <c r="B55" s="77" t="s">
         <v>117</v>
       </c>
       <c r="C55" s="47">
         <f>IF(Vout&gt;Vin_min, Vin_min^2*eff*(Vout-Vin_min)/(K*Ioutmax*fsw*Vout^2), (1-Vout/Vin_max)*Vout/(K*Ioutmax*fsw))</f>
-        <v>8.6420847367488022E-7</v>
+        <v>5.1852508420492811E-7</v>
       </c>
       <c r="D55" s="78" t="s">
         <v>5</v>
@@ -5483,7 +5495,7 @@
       <c r="P55" s="65"/>
       <c r="Q55" s="60"/>
     </row>
-    <row r="56" spans="1:17" ht="15.6" customHeight="1">
+    <row r="56" spans="1:17" ht="15.65" customHeight="1">
       <c r="A56" s="58"/>
       <c r="B56" s="77" t="s">
         <v>17</v>
@@ -5515,7 +5527,7 @@
       </c>
       <c r="C57" s="42">
         <f>IF(Vout&gt;Vin_min, ((Ioutmax/(Vin_min/Vout)/eff)^2+1/12*(Vin_min/L*(1-Vin_min/Vout)/fsw)^2)^0.5, ((Ioutmax^2+1/12*(Vout/L*(1-Vout/Vin_max)/fsw)^2)^0.5))</f>
-        <v>13.207992490615243</v>
+        <v>21.990736087604155</v>
       </c>
       <c r="D57" s="78" t="s">
         <v>19</v>
@@ -5543,7 +5555,7 @@
       </c>
       <c r="C58" s="42">
         <f>IF(Vout&gt;Vin_min, (Ioutmax/(Vin_min/Vout)/eff+(1/2*Vin_min/L*(1-Vin_min/Vout)/fsw)), Ioutmax+1/2*(Vout*(1-Vout/Vin_max)/L/fsw))</f>
-        <v>14.481830879632687</v>
+        <v>23.273039670841477</v>
       </c>
       <c r="D58" s="78" t="s">
         <v>4</v>
@@ -5571,7 +5583,7 @@
       </c>
       <c r="C59" s="42">
         <f>IF(Vout&gt;Vin_min, (Ioutmax/(Vin_min/Vout)/eff-(1/2*Vin_min/L*(1-Vin_min/Vout)/fsw)), Ioutmax-1/2*(Vout*(1-Vout/Vin_max)/L/fsw))</f>
-        <v>11.891795493993685</v>
+        <v>20.683004285202479</v>
       </c>
       <c r="D59" s="78" t="s">
         <v>4</v>
@@ -5617,7 +5629,7 @@
       <c r="P60" s="65"/>
       <c r="Q60" s="60"/>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" ht="13">
       <c r="A61" s="58"/>
       <c r="B61" s="80" t="s">
         <v>88</v>
@@ -5643,7 +5655,7 @@
       <c r="P61" s="65"/>
       <c r="Q61" s="60"/>
     </row>
-    <row r="62" spans="1:17" ht="26.4">
+    <row r="62" spans="1:17" ht="25">
       <c r="A62" s="58"/>
       <c r="B62" s="92" t="s">
         <v>105</v>
@@ -5722,7 +5734,7 @@
       <c r="P64" s="65"/>
       <c r="Q64" s="60"/>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" ht="13">
       <c r="A65" s="58"/>
       <c r="B65" s="80" t="s">
         <v>115</v>
@@ -5756,7 +5768,7 @@
         <v>223</v>
       </c>
       <c r="C66" s="37">
-        <v>0.1</v>
+        <v>12</v>
       </c>
       <c r="D66" s="78" t="s">
         <v>227</v>
@@ -5879,7 +5891,7 @@
       <c r="P70" s="65"/>
       <c r="Q70" s="60"/>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" ht="13">
       <c r="A71" s="58"/>
       <c r="B71" s="155" t="s">
         <v>298</v>
@@ -5987,7 +5999,7 @@
       </c>
       <c r="C75" s="53">
         <f>17+Ioutmax/2.5</f>
-        <v>18.2</v>
+        <v>19</v>
       </c>
       <c r="D75" s="78" t="s">
         <v>161</v>
@@ -6015,7 +6027,7 @@
       </c>
       <c r="C76" s="38">
         <f>IF((Op_mode="Buck"), Ioutmax/2/PI()/Vout_LP/(Cout_c+Cout_e), Ioutmax/PI()/Vout_LP/(Cout_c+Cout_e))</f>
-        <v>176.83882565766149</v>
+        <v>294.73137609610251</v>
       </c>
       <c r="D76" s="78" t="s">
         <v>6</v>
@@ -6043,7 +6055,7 @@
       </c>
       <c r="C77" s="38">
         <f>IF(Op_mode="Boost", Vout_LP*(eff*Vin_LP/Vout_LP)^2/2/PI()/L/Ioutmax, "No RPHZ")</f>
-        <v>14976.841860727107</v>
+        <v>8986.1051164362634</v>
       </c>
       <c r="D77" s="78" t="s">
         <v>6</v>
@@ -6146,14 +6158,14 @@
       <c r="P80" s="65"/>
       <c r="Q80" s="60"/>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" ht="13">
       <c r="A81" s="93"/>
       <c r="B81" s="80" t="s">
         <v>110</v>
       </c>
       <c r="C81" s="31">
         <f>IF(Op_mode="Boost", 2*PI()*fco*(Cout_c+Cout_e)*Vout_max/1.129/gm_PS/(eff*Vin_LP/Vout_LP)/gm_EA, 2*PI()*fco*(Cout_c+Cout_e)*Vout_max/1.129/gm_PS/gm_EA)</f>
-        <v>191004.36870310607</v>
+        <v>182962.0794945542</v>
       </c>
       <c r="D81" s="78" t="s">
         <v>28</v>
@@ -6199,7 +6211,7 @@
       <c r="P82" s="65"/>
       <c r="Q82" s="60"/>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" ht="13">
       <c r="A83" s="93"/>
       <c r="B83" s="80" t="s">
         <v>111</v>
@@ -6280,14 +6292,14 @@
       <c r="P85" s="65"/>
       <c r="Q85" s="60"/>
     </row>
-    <row r="86" spans="1:17" ht="26.4">
+    <row r="86" spans="1:17" ht="25.5">
       <c r="A86" s="93"/>
       <c r="B86" s="80" t="s">
         <v>113</v>
       </c>
       <c r="C86" s="54">
         <f>Ccomp*(IF(fzRHP&gt;fz_ESR, (Cout_e*ESR/Rcomp)/(Ccomp-Cout_e*ESR/Rcomp), (1/2/PI()/fzRHP/Rcomp)/(Ccomp-1/2/PI()/fzRHP/Rcomp)))</f>
-        <v>1.4470499188694438E-10</v>
+        <v>2.4464571751432752E-10</v>
       </c>
       <c r="D86" s="78" t="s">
         <v>9</v>
@@ -6361,7 +6373,7 @@
       <c r="P88" s="65"/>
       <c r="Q88" s="60"/>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" ht="13">
       <c r="A89" s="93"/>
       <c r="B89" s="151" t="s">
         <v>329</v>
@@ -6416,7 +6428,7 @@
       </c>
       <c r="C91" s="56">
         <f>IF(Vin_eff&lt;Vout, ((Ioutmax/(Vin_eff/Vout)/eff)^2+1/12*(Vin_eff/L*(1-Vin_eff/Vout)/fsw)^2)^0.5, ((Ioutmax^2+1/12*(Vout/L*(1-Vout/Vin_eff)/fsw)^2)^0.5))</f>
-        <v>10.725777315708788</v>
+        <v>17.840298245653148</v>
       </c>
       <c r="D91" s="78" t="s">
         <v>4</v>
@@ -6444,7 +6456,7 @@
       </c>
       <c r="C92" s="56">
         <f>IF(Vin_eff&lt;Vout, (Ioutmax/(Vin_eff/Vout)/eff+(1/2*Vin_eff/L*(1-Vin_eff/Vout)/fsw)), Ioutmax+1/2*(Vout*(1-Vout/Vin_eff)/L/fsw))</f>
-        <v>12.164973408547244</v>
+        <v>19.292980536554367</v>
       </c>
       <c r="D92" s="78" t="s">
         <v>4</v>
@@ -6472,7 +6484,7 @@
       </c>
       <c r="C93" s="56">
         <f>IF(Vin_eff&lt;Vout, (Ioutmax/(Vin_eff/Vout)/eff-(1/2*Vin_eff/L*(1-Vin_eff/Vout)/fsw)),Ioutmax-1/2*(Vout*(1-Vout/Vin_eff)/L/fsw))</f>
-        <v>9.2190479754741403</v>
+        <v>16.347055103481267</v>
       </c>
       <c r="D93" s="78" t="s">
         <v>4</v>
@@ -6790,7 +6802,7 @@
       <c r="P104" s="65"/>
       <c r="Q104" s="60"/>
     </row>
-    <row r="105" spans="1:17" ht="26.4">
+    <row r="105" spans="1:17" ht="25">
       <c r="A105" s="58"/>
       <c r="B105" s="77" t="s">
         <v>69</v>
@@ -6871,7 +6883,7 @@
       <c r="P107" s="65"/>
       <c r="Q107" s="60"/>
     </row>
-    <row r="108" spans="1:17" ht="26.4">
+    <row r="108" spans="1:17" ht="25">
       <c r="A108" s="58"/>
       <c r="B108" s="77" t="s">
         <v>72</v>
@@ -7040,7 +7052,7 @@
       </c>
       <c r="C114" s="31">
         <f>Rpcb*(ILrms^2)</f>
-        <v>230.08459805234642</v>
+        <v>636.5524829877096</v>
       </c>
       <c r="D114" s="78" t="s">
         <v>10</v>
@@ -7068,7 +7080,7 @@
       </c>
       <c r="C115" s="31">
         <f>(ILrms)^2*DCR*1000</f>
-        <v>293.3578625167417</v>
+        <v>811.60441580932979</v>
       </c>
       <c r="D115" s="78" t="s">
         <v>10</v>
@@ -7089,7 +7101,7 @@
       <c r="P115" s="65"/>
       <c r="Q115" s="60"/>
     </row>
-    <row r="116" spans="1:17" ht="37.799999999999997" customHeight="1">
+    <row r="116" spans="1:17" ht="37.75" customHeight="1">
       <c r="A116" s="93"/>
       <c r="B116" s="77" t="s">
         <v>275</v>
@@ -7123,7 +7135,7 @@
       </c>
       <c r="C117" s="31">
         <f>IF(Vin_eff&lt;Vout, ((0.001+0.00000001*fsw)*IF(AND(Vout&gt;Vin_eff, Vin_eff&gt;6.2), Vin_eff, Vout)+(1-Vin_eff/Vout)*ILrms^2*BST_LS_Rdson+(Vin_eff/Vout)*ILrms^2*BST_HS_Rdson+1/2*ILpeak*(Vout+BST_HS_Vd)*BST_LS_rise_time*fsw+1/2*ILvalley*(Vout+BST_HS_Vd)*BST_LS_fall_time*fsw+1/2*0.0000000005*(Vout+BST_HS_Vd)*(Vout+BST_HS_Vd)*fsw+(ILpeak+ILvalley)*BST_HS_Vd*BST_HS_dead_time*fsw+Vout*0.000000005*fsw)*1000, ((0.001+(BUCK_HS_Qg+BUCK_LS_Qg)*fsw)*IF(AND(Vin_eff&gt;Vout, Vout&gt;6.2), Vout, Vin_eff)+BST_HS_Rdson*ILrms^2)*1000)</f>
-        <v>1816.6843091008059</v>
+        <v>3879.2361605840729</v>
       </c>
       <c r="D117" s="78" t="s">
         <v>10</v>
@@ -7151,7 +7163,7 @@
       </c>
       <c r="C118" s="32">
         <f>Ioutmax*Ioutmax*R_1</f>
-        <v>90</v>
+        <v>250</v>
       </c>
       <c r="D118" s="78" t="s">
         <v>10</v>
@@ -7207,7 +7219,7 @@
       </c>
       <c r="C120" s="32">
         <f>IF(Vin_eff&lt;Vout, (ILrms)^2*(BUCK_HS_Rdson)*1000, ((Vout/Vin_eff)*ILrms^2*BUCK_HS_Rdson+1/2*ILpeak*(Vin_eff+BUCK_LS_Vd)*BUCK_HS_fall_time*fsw+1/2*ILvalley*(Vin_eff+BUCK_LS_Vd)*BUCK_HS_rise_time*fsw+1/2*BUCK_HS_Coss*(Vin_eff+BUCK_LS_Vd)*(Vin_eff+BUCK_LS_Vd)*fsw)*1000)</f>
-        <v>747.77494367012582</v>
+        <v>2068.795569710056</v>
       </c>
       <c r="D120" s="78" t="s">
         <v>10</v>
@@ -7263,7 +7275,7 @@
       </c>
       <c r="C122" s="32">
         <f>IF(Vin_eff&lt;Vout, 1000*ESR*(G122+H122), 0)</f>
-        <v>176.35927283606784</v>
+        <v>489.88686898907707</v>
       </c>
       <c r="D122" s="96" t="s">
         <v>10</v>
@@ -7277,11 +7289,11 @@
       </c>
       <c r="G122" s="112">
         <f>(fsw*(Cout_e/(Cout_c+Cout_e))^2*(Ioutmax^2*(Vout-Vin_eff)/Vout/fsw+2*Ioutmax*((1-EXP((-Vin_eff/Vout)/tou/fsw))/(1-EXP(-1/tou/fsw))*(ILpeak+ILvalley)/2*tou*(EXP(-1/tou*(1-Vin_eff/Vout)/fsw)-1))-((1-EXP((-Vin_eff/Vout)/tou/fsw))/(1-EXP(-1/tou/fsw))*(ILpeak+ILvalley)/2)^2*tou/2*(EXP(-2/tou*(1-Vin_eff/Vout)/fsw)-1)))</f>
-        <v>5.7188731757709901</v>
+        <v>15.885758821586084</v>
       </c>
       <c r="H122" s="112">
         <f>(fsw*(Cout_e/(Cout_c+Cout_e))^2*((((ILpeak+ILvalley)/2-Ioutmax)^2*Vin_eff/Vout/fsw+2*((ILpeak+ILvalley)/2-Ioutmax)*((1-EXP(-(1-Vin_eff/Vout)/tou/fsw))/(1-EXP(-1/tou/fsw))*(ILpeak+ILvalley)/2*tou*(EXP(-1/tou*(Vin_eff/Vout)/fsw)-1))-((1-EXP(-(1-Vin_eff/Vout)/tou/fsw))/(1-EXP(-1/tou/fsw))*(ILpeak+ILvalley)/2)^2*tou/2*(EXP(-2/tou*(1-Vin_eff/Vout/fsw))-1))))</f>
-        <v>13.876601583792102</v>
+        <v>38.546115510533596</v>
       </c>
       <c r="I122" s="64"/>
       <c r="J122" s="64"/>
@@ -7293,14 +7305,14 @@
       <c r="P122" s="65"/>
       <c r="Q122" s="60"/>
     </row>
-    <row r="123" spans="1:17" ht="13.8">
+    <row r="123" spans="1:17" ht="13">
       <c r="A123" s="93"/>
       <c r="B123" s="95" t="s">
         <v>325</v>
       </c>
       <c r="C123" s="33">
         <f>IF(Vin_eff&lt;Vout, Vout*Ioutmax/(Vout*Ioutmax+(C114+C115+C116+C117+C118+C119+C120+C121+C122)/1000), Vout*Ioutmax/(Vout*Ioutmax+(C114+C115+C116+C117+C118+C119+C120+C121)/1000))</f>
-        <v>0.90684073069437698</v>
+        <v>0.87616725833898967</v>
       </c>
       <c r="D123" s="96"/>
       <c r="E123" s="100" t="s">
@@ -7319,7 +7331,7 @@
       <c r="P123" s="65"/>
       <c r="Q123" s="60"/>
     </row>
-    <row r="124" spans="1:17" ht="26.4">
+    <row r="124" spans="1:17" ht="25">
       <c r="A124" s="93"/>
       <c r="B124" s="77" t="s">
         <v>316</v>
@@ -7346,14 +7358,14 @@
       <c r="P124" s="65"/>
       <c r="Q124" s="60"/>
     </row>
-    <row r="125" spans="1:17" ht="27" thickBot="1">
+    <row r="125" spans="1:17" ht="25.5" thickBot="1">
       <c r="A125" s="93"/>
       <c r="B125" s="101" t="s">
         <v>81</v>
       </c>
       <c r="C125" s="34">
         <f>C124*(C117)/1000</f>
-        <v>67.217319436729809</v>
+        <v>143.53173794161069</v>
       </c>
       <c r="D125" s="102" t="s">
         <v>86</v>
@@ -7374,7 +7386,7 @@
       <c r="P125" s="105"/>
       <c r="Q125" s="60"/>
     </row>
-    <row r="126" spans="1:17" ht="13.8" thickTop="1">
+    <row r="126" spans="1:17" ht="13" thickTop="1">
       <c r="A126" s="93"/>
       <c r="B126" s="60"/>
       <c r="C126" s="106"/>
@@ -7601,15 +7613,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>53340</xdr:colOff>
+                <xdr:colOff>50800</xdr:colOff>
                 <xdr:row>12</xdr:row>
                 <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>15</xdr:col>
-                <xdr:colOff>220980</xdr:colOff>
+                <xdr:colOff>222250</xdr:colOff>
                 <xdr:row>30</xdr:row>
-                <xdr:rowOff>175260</xdr:rowOff>
+                <xdr:rowOff>177800</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7631,33 +7643,33 @@
       <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="8.21875" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" customWidth="1"/>
-    <col min="13" max="14" width="8.44140625" customWidth="1"/>
-    <col min="15" max="16" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.90625" customWidth="1"/>
+    <col min="8" max="8" width="8.36328125" customWidth="1"/>
+    <col min="9" max="9" width="8.1796875" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" customWidth="1"/>
+    <col min="13" max="14" width="8.453125" customWidth="1"/>
+    <col min="15" max="16" width="9.54296875" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" customWidth="1"/>
-    <col min="19" max="20" width="9.44140625" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" customWidth="1"/>
+    <col min="19" max="20" width="9.453125" customWidth="1"/>
     <col min="21" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="10.109375" customWidth="1"/>
+    <col min="24" max="24" width="10.08984375" customWidth="1"/>
     <col min="25" max="26" width="10" customWidth="1"/>
-    <col min="27" max="29" width="10.33203125" customWidth="1"/>
-    <col min="30" max="30" width="10.21875" customWidth="1"/>
-    <col min="32" max="32" width="15.77734375" customWidth="1"/>
-    <col min="33" max="33" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5546875" customWidth="1"/>
+    <col min="27" max="29" width="10.36328125" customWidth="1"/>
+    <col min="30" max="30" width="10.1796875" customWidth="1"/>
+    <col min="32" max="32" width="15.81640625" customWidth="1"/>
+    <col min="33" max="33" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="14.4" thickTop="1" thickBot="1">
+    <row r="1" spans="1:34" ht="14" thickTop="1" thickBot="1">
       <c r="A1" s="158" t="s">
         <v>176</v>
       </c>
@@ -7703,7 +7715,7 @@
       <c r="AC1" s="159"/>
       <c r="AD1" s="160"/>
     </row>
-    <row r="2" spans="1:34" ht="27" thickTop="1">
+    <row r="2" spans="1:34" ht="25.5" thickTop="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>171</v>
@@ -7812,19 +7824,19 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C43" si="0">20*LOG(SQRT((B3/fzRHP)^2+1))</f>
-        <v>1.9361283416929328E-4</v>
+        <v>5.3779211746001658E-4</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" ref="D3:D43" si="1">-180/PI()*ATAN(B3/fzRHP)</f>
-        <v>-0.38255680747145937</v>
+        <v>-0.63757783598200435</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" ref="E3:E43" si="2">20*LOG(1/SQRT((B3/fp)^2+1))</f>
-        <v>-1.2049995751356051</v>
+        <v>-0.47321241223349364</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F43" si="3">-180/PI()*ATAN(B3/fp)</f>
-        <v>-29.487580957512936</v>
+        <v>-18.741663749715418</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G43" si="4">20*LOG(SQRT((B3/fz_ESR)^2+1))</f>
@@ -7884,11 +7896,11 @@
       </c>
       <c r="U3" s="5">
         <f t="shared" ref="U3:U43" si="16">20*LOG(1/SQRT((2*PI()*B3*R_ca*C_ca)^2+(1-(2*PI()*B3)^2*C_ca/gm_ca/(IF(Op_mode="Boost", Vout_LP, Vin_LP)/V_m/L)*gm_PS)^2))</f>
-        <v>-6.0025299636997711E-5</v>
+        <v>-5.9710471568700182E-5</v>
       </c>
       <c r="V3" s="15">
         <f t="shared" ref="V3:V43" si="17">IF(-180/PI()*ATAN((2*PI()*B3*R_ca*C_ca)/(1-(2*PI()*B3)^2*C_ca/gm_ca/(IF(Op_mode="Boost", Vout_LP, Vin_LP)/V_m/L)*gm_PS))&gt;0, -180/PI()*ATAN((2*PI()*B3*R_ca*C_ca)/(1-(2*PI()*B3)^2*C_ca/gm_ca/(IF(Op_mode="Boost", Vout_LP, Vin_LP)/V_m/L)*gm_PS))-180, -180/PI()*ATAN((2*PI()*B3*R_ca*C_ca)/(1-(2*PI()*B3)^2*C_ca/gm_ca/(IF(Op_mode="Boost", Vout_LP, Vin_LP)/V_m/L)*gm_PS)))</f>
-        <v>-0.22535902368664043</v>
+        <v>-0.22535903185502804</v>
       </c>
       <c r="W3" s="12">
         <v>0</v>
@@ -7907,19 +7919,19 @@
       </c>
       <c r="AA3" s="5">
         <f t="shared" ref="AA3:AA43" si="19">IF(Op_mode="Boost", C3+E3+G3+I3+K3+M3+20*LOG(Vout_LP/Ioutmax/2*gm_PS*eff*Vin_LP/Vout_LP*gm_EA*10000000*1.129/Vout_max)+Q3+S3+U3+Y3, E3+G3+I3+K3+M3+20*LOG(Vout_LP/Ioutmax*gm_PS*gm_EA*10000000*1.129/Vout_max)+Q3+S3+U3+Y3)</f>
-        <v>25.464873663838915</v>
+        <v>22.133674587880346</v>
       </c>
       <c r="AB3" s="5">
         <f t="shared" ref="AB3:AB43" si="20">IF(Op_mode="Boost", D3+F3+H3+J3+180+L3+N3+R3+T3+V3+X3+Z3, F3+H3+J3+180+L3+N3+R3+T3+V3+Z3)</f>
-        <v>79.693197380990057</v>
+        <v>90.184093552108635</v>
       </c>
       <c r="AC3" s="5">
         <f>AA3+O3</f>
-        <v>25.464769014426569</v>
+        <v>22.133569938468</v>
       </c>
       <c r="AD3" s="6">
         <f>AB3+P3</f>
-        <v>79.41194383824508</v>
+        <v>89.902840009363658</v>
       </c>
       <c r="AF3" t="s">
         <v>179</v>
@@ -7931,7 +7943,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="13.8">
+    <row r="4" spans="1:34" ht="13">
       <c r="A4" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -7941,19 +7953,19 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>3.0685166232814634E-4</v>
+        <v>8.5231220192058727E-4</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="1"/>
-        <v>-0.48160630049671649</v>
+        <v>-0.80264356300382855</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="2"/>
-        <v>-1.7805835252755517</v>
+        <v>-0.72783308484928044</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="3"/>
-        <v>-35.44727475487106</v>
+        <v>-23.129427552061749</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="4"/>
@@ -8013,11 +8025,11 @@
       </c>
       <c r="U4" s="5">
         <f t="shared" si="16"/>
-        <v>-9.5133306981339747E-5</v>
+        <v>-9.4634342386585882E-5</v>
       </c>
       <c r="V4" s="15">
         <f t="shared" si="17"/>
-        <v>-0.28370948281009239</v>
+        <v>-0.283709499108037</v>
       </c>
       <c r="W4" s="12">
         <v>0</v>
@@ -8036,19 +8048,19 @@
       </c>
       <c r="AA4" s="5">
         <f t="shared" si="19"/>
-        <v>23.131521325899396</v>
+        <v>20.121486992857815</v>
       </c>
       <c r="AB4" s="5">
         <f t="shared" si="20"/>
-        <v>77.65850866947649</v>
+        <v>89.655318593480743</v>
       </c>
       <c r="AC4" s="5">
         <f t="shared" ref="AC4:AC43" si="26">AA4+O4</f>
-        <v>23.131355468926941</v>
+        <v>20.12132113588536</v>
       </c>
       <c r="AD4" s="6">
         <f t="shared" ref="AD4:AD43" si="27">AB4+P4</f>
-        <v>77.304433100763788</v>
+        <v>89.301243024768041</v>
       </c>
       <c r="AF4" t="s">
         <v>177</v>
@@ -8070,19 +8082,19 @@
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>4.8631706231723346E-4</v>
+        <v>1.3507462894831834E-3</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="1"/>
-        <v>-0.60629805857672359</v>
+        <v>-1.0104297208000355</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="2"/>
-        <v>-2.5605327771769613</v>
+        <v>-1.103088495418898</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="3"/>
-        <v>-41.867838901620914</v>
+        <v>-28.268768005153763</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="4"/>
@@ -8142,11 +8154,11 @@
       </c>
       <c r="U5" s="5">
         <f t="shared" si="16"/>
-        <v>-1.507751716112957E-4</v>
+        <v>-1.4998437674752164E-4</v>
       </c>
       <c r="V5" s="15">
         <f t="shared" si="17"/>
-        <v>-0.35716764312809113</v>
+        <v>-0.35716767564635021</v>
       </c>
       <c r="W5" s="12">
         <v>0</v>
@@ -8165,19 +8177,19 @@
       </c>
       <c r="AA5" s="5">
         <f t="shared" si="19"/>
-        <v>20.709173293763662</v>
+        <v>18.104152062571714</v>
       </c>
       <c r="AB5" s="5">
         <f t="shared" si="20"/>
-        <v>75.948012118873066</v>
+        <v>89.142951320598641</v>
       </c>
       <c r="AC5" s="5">
         <f t="shared" si="26"/>
-        <v>20.708910431112834</v>
+        <v>18.103889199920886</v>
       </c>
       <c r="AD5" s="6">
         <f t="shared" si="27"/>
-        <v>75.50226070658411</v>
+        <v>88.697199908309685</v>
       </c>
       <c r="AF5" t="s">
         <v>178</v>
@@ -8199,19 +8211,19 @@
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>7.7073536279571723E-4</v>
+        <v>2.1405939230661362E-3</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="1"/>
-        <v>-0.76326737050132176</v>
+        <v>-1.2719785346634249</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="2"/>
-        <v>-3.5660859375118523</v>
+        <v>-1.6384605841639688</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="3"/>
-        <v>-48.449633597167093</v>
+        <v>-34.097079115107846</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="4"/>
@@ -8271,11 +8283,11 @@
       </c>
       <c r="U6" s="5">
         <f t="shared" si="16"/>
-        <v>-2.3896013423831418E-4</v>
+        <v>-2.377068357733286E-4</v>
       </c>
       <c r="V6" s="15">
         <f t="shared" si="17"/>
-        <v>-0.44964456035969824</v>
+        <v>-0.44964462524084126</v>
       </c>
       <c r="W6" s="12">
         <v>0</v>
@@ -8294,19 +8306,19 @@
       </c>
       <c r="AA6" s="5">
         <f t="shared" si="19"/>
-        <v>18.215899243851148</v>
+        <v>16.081564976085726</v>
       </c>
       <c r="AB6" s="5">
         <f t="shared" si="20"/>
-        <v>74.794541988552837</v>
+        <v>88.638385241568827</v>
       </c>
       <c r="AC6" s="5">
         <f t="shared" si="26"/>
-        <v>18.215482641999262</v>
+        <v>16.081148374233841</v>
       </c>
       <c r="AD6" s="6">
         <f t="shared" si="27"/>
-        <v>74.233380830043899</v>
+        <v>88.077224083059889</v>
       </c>
       <c r="AF6" t="s">
         <v>180</v>
@@ -8329,19 +8341,19 @@
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>1.2214698402175032E-3</v>
+        <v>3.392123886011207E-3</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="1"/>
-        <v>-0.96086344591115713</v>
+        <v>-1.6011722739270928</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="2"/>
-        <v>-4.7966814749016438</v>
+        <v>-2.3712940260555793</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="3"/>
-        <v>-54.854146294158951</v>
+        <v>-40.439726667075412</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="4"/>
@@ -8401,11 +8413,11 @@
       </c>
       <c r="U7" s="5">
         <f t="shared" si="16"/>
-        <v>-3.7872023949901202E-4</v>
+        <v>-3.7673396294243269E-4</v>
       </c>
       <c r="V7" s="15">
         <f t="shared" si="17"/>
-        <v>-0.56606325335972674</v>
+        <v>-0.56606338281047131</v>
       </c>
       <c r="W7" s="12">
         <v>0</v>
@@ -8424,19 +8436,19 @@
       </c>
       <c r="AA7" s="5">
         <f t="shared" si="19"/>
-        <v>15.690578878369591</v>
+        <v>14.054808234565964</v>
       </c>
       <c r="AB7" s="5">
         <f t="shared" si="20"/>
-        <v>74.360877756745992</v>
+        <v>88.134988426362867</v>
       </c>
       <c r="AC7" s="5">
         <f t="shared" si="26"/>
-        <v>15.689918627452</v>
+        <v>14.054147983648374</v>
       </c>
       <c r="AD7" s="6">
         <f t="shared" si="27"/>
-        <v>73.654430925619607</v>
+        <v>87.428541595236481</v>
       </c>
     </row>
     <row r="8" spans="1:34">
@@ -8449,19 +8461,19 @@
       </c>
       <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>1.9357400358919379E-3</v>
+        <v>5.374926727589757E-3</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="1"/>
-        <v>-1.2095890918780396</v>
+        <v>-2.0154496769777892</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="2"/>
-        <v>-6.2301675920942259</v>
+        <v>-3.3267890307115602</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="3"/>
-        <v>-60.78549163251769</v>
+        <v>-47.015101279175312</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="4"/>
@@ -8521,11 +8533,11 @@
       </c>
       <c r="U8" s="5">
         <f t="shared" si="16"/>
-        <v>-6.0021593203675992E-4</v>
+        <v>-5.9706806576454103E-4</v>
       </c>
       <c r="V8" s="15">
         <f t="shared" si="17"/>
-        <v>-0.71262002205161468</v>
+        <v>-0.71262028032666902</v>
       </c>
       <c r="W8" s="12">
         <v>0</v>
@@ -8544,19 +8556,19 @@
       </c>
       <c r="AA8" s="5">
         <f t="shared" si="19"/>
-        <v>13.18293807129966</v>
+        <v>12.026428234268257</v>
       </c>
       <c r="AB8" s="5">
         <f t="shared" si="20"/>
-        <v>74.656766089510825</v>
+        <v>87.621295599478401</v>
       </c>
       <c r="AC8" s="5">
         <f t="shared" si="26"/>
-        <v>13.18189169063429</v>
+        <v>12.025381853602887</v>
       </c>
       <c r="AD8" s="6">
         <f t="shared" si="27"/>
-        <v>73.767428579704003</v>
+        <v>86.731958089671579</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -8569,19 +8581,19 @@
       </c>
       <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>3.0675414296031677E-3</v>
+        <v>8.5156042976694563E-3</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="1"/>
-        <v>-1.5226501586426631</v>
+        <v>-2.536689126510864</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="2"/>
-        <v>-7.8305237849889187</v>
+        <v>-4.5094376799833205</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="3"/>
-        <v>-66.04925313079822</v>
+        <v>-53.486278866564746</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="4"/>
@@ -8641,11 +8653,11 @@
       </c>
       <c r="U9" s="5">
         <f t="shared" si="16"/>
-        <v>-9.5123997391355591E-4</v>
+        <v>-9.4625136884671451E-4</v>
       </c>
       <c r="V9" s="15">
         <f t="shared" si="17"/>
-        <v>-0.89711272590656244</v>
+        <v>-0.89711324119150393</v>
       </c>
       <c r="W9" s="12">
         <v>0</v>
@@ -8664,19 +8676,19 @@
       </c>
       <c r="AA9" s="5">
         <f t="shared" si="19"/>
-        <v>10.736754899210808</v>
+        <v>9.9999633227175018</v>
       </c>
       <c r="AB9" s="5">
         <f t="shared" si="20"/>
-        <v>75.52481805965347</v>
+        <v>87.073752840733789</v>
       </c>
       <c r="AC9" s="5">
         <f t="shared" si="26"/>
-        <v>10.735096614450665</v>
+        <v>9.9983050379573584</v>
       </c>
       <c r="AD9" s="6">
         <f t="shared" si="27"/>
-        <v>74.405261052728335</v>
+        <v>85.954195833808654</v>
       </c>
     </row>
     <row r="10" spans="1:34">
@@ -8689,19 +8701,19 @@
       </c>
       <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>4.8607217891385879E-3</v>
+        <v>1.3488595091278262E-2</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="1"/>
-        <v>-1.9166391374638205</v>
+        <v>-3.1922832926385398</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="2"/>
-        <v>-9.5580265351730951</v>
+        <v>-5.9013491199998978</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="3"/>
-        <v>-70.565128107755442</v>
+        <v>-59.541644560656373</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="4"/>
@@ -8761,11 +8773,11 @@
       </c>
       <c r="U10" s="5">
         <f t="shared" si="16"/>
-        <v>-1.5075178916900789E-3</v>
+        <v>-1.4996125572330895E-3</v>
       </c>
       <c r="V10" s="15">
         <f t="shared" si="17"/>
-        <v>-1.1293526636173239</v>
+        <v>-1.1293536916146123</v>
       </c>
       <c r="W10" s="12">
         <v>0</v>
@@ -8784,19 +8796,19 @@
       </c>
       <c r="AA10" s="5">
         <f t="shared" si="19"/>
-        <v>8.3769342992349962</v>
+        <v>7.9789167600727495</v>
       </c>
       <c r="AB10" s="5">
         <f t="shared" si="20"/>
-        <v>76.705922221255562</v>
+        <v>86.453760585182621</v>
       </c>
       <c r="AC10" s="5">
         <f t="shared" si="26"/>
-        <v>8.3743063884077866</v>
+        <v>7.976288849245539</v>
       </c>
       <c r="AD10" s="6">
         <f t="shared" si="27"/>
-        <v>75.296588350902027</v>
+        <v>85.044426714829086</v>
       </c>
     </row>
     <row r="11" spans="1:34">
@@ -8809,19 +8821,19 @@
       </c>
       <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>7.7012053855227813E-3</v>
+        <v>2.1358608446179643E-2</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="1"/>
-        <v>-2.4123796212611062</v>
+        <v>-4.0164184265513256</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="2"/>
-        <v>-11.376856982343668</v>
+        <v>-7.4686549282649075</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="3"/>
-        <v>-74.343374771426397</v>
+        <v>-64.961886892073892</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="4"/>
@@ -8881,11 +8893,11 @@
       </c>
       <c r="U11" s="5">
         <f t="shared" si="16"/>
-        <v>-2.3890140890865199E-3</v>
+        <v>-2.3764876695548439E-3</v>
       </c>
       <c r="V11" s="15">
         <f t="shared" si="17"/>
-        <v>-1.421680311293352</v>
+        <v>-1.4216823620024142</v>
       </c>
       <c r="W11" s="12">
         <v>0</v>
@@ -8904,19 +8916,19 @@
       </c>
       <c r="AA11" s="5">
         <f t="shared" si="19"/>
-        <v>6.1074461994846878</v>
+        <v>5.9659874500715979</v>
       </c>
       <c r="AB11" s="5">
         <f t="shared" si="20"/>
-        <v>77.933027958115034</v>
+        <v>85.710474981468266</v>
       </c>
       <c r="AC11" s="5">
         <f t="shared" si="26"/>
-        <v>6.1032819782090266</v>
+        <v>5.9618232287959367</v>
       </c>
       <c r="AD11" s="6">
         <f t="shared" si="27"/>
-        <v>76.158990956845713</v>
+        <v>83.936437980198946</v>
       </c>
     </row>
     <row r="12" spans="1:34">
@@ -8929,19 +8941,19 @@
       </c>
       <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>1.2199266446766978E-2</v>
+        <v>3.3802599206686539E-2</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="1"/>
-        <v>-3.0359573761506455</v>
+        <v>-5.0515400436283073</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="2"/>
-        <v>-13.25853157242139</v>
+        <v>-9.1716518773164033</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="3"/>
-        <v>-77.449099446690596</v>
+        <v>-69.642888982717182</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="4"/>
@@ -9001,11 +9013,11 @@
       </c>
       <c r="U12" s="5">
         <f t="shared" si="16"/>
-        <v>-3.7857276280555048E-3</v>
+        <v>-3.7658813475650124E-3</v>
       </c>
       <c r="V12" s="15">
         <f t="shared" si="17"/>
-        <v>-1.7896090448466262</v>
+        <v>-1.7896131352368827</v>
       </c>
       <c r="W12" s="12">
         <v>0</v>
@@ -9024,19 +9036,19 @@
       </c>
       <c r="AA12" s="5">
         <f t="shared" si="19"/>
-        <v>3.9179831647260186</v>
+        <v>3.9631553058993743</v>
       </c>
       <c r="AB12" s="5">
         <f t="shared" si="20"/>
-        <v>78.995038517174109</v>
+        <v>84.785662223279616</v>
       </c>
       <c r="AC12" s="5">
         <f t="shared" si="26"/>
-        <v>3.9113851681655283</v>
+        <v>3.9565573093388839</v>
       </c>
       <c r="AD12" s="6">
         <f t="shared" si="27"/>
-        <v>76.762075478306571</v>
+        <v>82.552699184412077</v>
       </c>
     </row>
     <row r="13" spans="1:34">
@@ -9049,19 +9061,19 @@
       </c>
       <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>1.9318683648281119E-2</v>
+        <v>5.3452247263486768E-2</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="1"/>
-        <v>-3.8199549503312737</v>
+        <v>-6.3499153331098181</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="2"/>
-        <v>-15.182179694787163</v>
+        <v>-10.973234928453262</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="3"/>
-        <v>-79.971560240179642</v>
+        <v>-73.578100650015031</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="4"/>
@@ -9121,11 +9133,11 @@
       </c>
       <c r="U13" s="5">
         <f t="shared" si="16"/>
-        <v>-5.9984562525295425E-3</v>
+        <v>-5.9670189753638844E-3</v>
       </c>
       <c r="V13" s="15">
         <f t="shared" si="17"/>
-        <v>-2.2526244843668004</v>
+        <v>-2.2526326416220468</v>
       </c>
       <c r="W13" s="12">
         <v>0</v>
@@ -9144,19 +9156,19 @@
       </c>
       <c r="AA13" s="5">
         <f t="shared" si="19"/>
-        <v>1.7927165877129916</v>
+        <v>1.9724956219672161</v>
       </c>
       <c r="AB13" s="5">
         <f t="shared" si="20"/>
-        <v>79.752830103810311</v>
+        <v>83.616321153941144</v>
       </c>
       <c r="AC13" s="5">
         <f t="shared" si="26"/>
-        <v>1.7822641088583582</v>
+        <v>1.9620431431125827</v>
       </c>
       <c r="AD13" s="6">
         <f t="shared" si="27"/>
-        <v>76.942527937914832</v>
+        <v>80.806018988045665</v>
       </c>
     </row>
     <row r="14" spans="1:34">
@@ -9169,19 +9181,19 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="0"/>
-        <v>3.0578347275027704E-2</v>
+        <v>8.4413866365830467E-2</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="1"/>
-        <v>-4.8048809496734659</v>
+        <v>-7.9750551930242617</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="2"/>
-        <v>-17.133304966826461</v>
+        <v>-12.843211280126624</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="3"/>
-        <v>-82.004088274730336</v>
+        <v>-76.823595298422575</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="4"/>
@@ -9241,11 +9253,11 @@
       </c>
       <c r="U14" s="5">
         <f t="shared" si="16"/>
-        <v>-9.5031035385685133E-3</v>
+        <v>-9.4533213520605584E-3</v>
       </c>
       <c r="V14" s="15">
         <f t="shared" si="17"/>
-        <v>-2.8351688373470472</v>
+        <v>-2.8351851001164667</v>
       </c>
       <c r="W14" s="12">
         <v>0</v>
@@ -9264,19 +9276,19 @@
       </c>
       <c r="AA14" s="5">
         <f t="shared" si="19"/>
-        <v>-0.28335809222699648</v>
+        <v>-2.7098372218994299E-3</v>
       </c>
       <c r="AB14" s="5">
         <f t="shared" si="20"/>
-        <v>80.123898825236822</v>
+        <v>82.134201295424361</v>
       </c>
       <c r="AC14" s="5">
         <f t="shared" si="26"/>
-        <v>-0.29991251500629795</v>
+        <v>-1.9264260001200916E-2</v>
       </c>
       <c r="AD14" s="6">
         <f t="shared" si="27"/>
-        <v>76.587595286264232</v>
+        <v>78.597897756451772</v>
       </c>
     </row>
     <row r="15" spans="1:34">
@@ -9289,19 +9301,19 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="0"/>
-        <v>4.8364129172934207E-2</v>
+        <v>0.1330370147863576</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="1"/>
-        <v>-6.0407248436563163</v>
+        <v>-10.002476022139833</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="2"/>
-        <v>-19.102181668409781</v>
+        <v>-14.759122626526374</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="3"/>
-        <v>-83.633398893403282</v>
+        <v>-79.465445201752047</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="4"/>
@@ -9361,11 +9373,11 @@
       </c>
       <c r="U15" s="5">
         <f t="shared" si="16"/>
-        <v>-1.505184972000863E-2</v>
+        <v>-1.4973056906153377E-2</v>
       </c>
       <c r="V15" s="15">
         <f t="shared" si="17"/>
-        <v>-3.5678365388988129</v>
+        <v>-3.5678689460667985</v>
       </c>
       <c r="W15" s="12">
         <v>0</v>
@@ -9384,19 +9396,19 @@
       </c>
       <c r="AA15" s="5">
         <f t="shared" si="19"/>
-        <v>-2.3212645940589907</v>
+        <v>-1.9567846067203545</v>
       </c>
       <c r="AB15" s="5">
         <f t="shared" si="20"/>
-        <v>80.057893416516862</v>
+        <v>80.264063522516608</v>
       </c>
       <c r="AC15" s="5">
         <f t="shared" si="26"/>
-        <v>-2.3474724188215106</v>
+        <v>-1.9829924314828746</v>
       </c>
       <c r="AD15" s="6">
         <f t="shared" si="27"/>
-        <v>75.609250528980056</v>
+        <v>75.815420634979802</v>
       </c>
     </row>
     <row r="16" spans="1:34">
@@ -9409,19 +9421,19 @@
       </c>
       <c r="C16" s="12">
         <f t="shared" si="0"/>
-        <v>7.6404335961211836E-2</v>
+        <v>0.20900147012647197</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="1"/>
-        <v>-7.588441507527774</v>
+        <v>-12.518782338090999</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>-21.082428808677061</v>
+        <v>-16.705216124384364</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="3"/>
-        <v>-84.935145713747275</v>
+        <v>-81.59728325390752</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="4"/>
@@ -9481,11 +9493,11 @@
       </c>
       <c r="U16" s="5">
         <f t="shared" si="16"/>
-        <v>-2.3831627181822329E-2</v>
+        <v>-2.3707015964796425E-2</v>
       </c>
       <c r="V16" s="15">
         <f t="shared" si="17"/>
-        <v>-4.4887933632545707</v>
+        <v>-4.4888578938085617</v>
       </c>
       <c r="W16" s="12">
         <v>0</v>
@@ -9504,19 +9516,19 @@
       </c>
       <c r="AA16" s="5">
         <f t="shared" si="19"/>
-        <v>-4.3269463659764886</v>
+        <v>-3.8803426692735363</v>
       </c>
       <c r="AB16" s="5">
         <f t="shared" si="20"/>
-        <v>79.51572656240495</v>
+        <v>77.923183661127496</v>
       </c>
       <c r="AC16" s="5">
         <f t="shared" si="26"/>
-        <v>-4.3684099841019499</v>
+        <v>-3.9218062873989981</v>
       </c>
       <c r="AD16" s="6">
         <f t="shared" si="27"/>
-        <v>73.921777727361587</v>
+        <v>72.329234826084132</v>
       </c>
     </row>
     <row r="17" spans="1:30">
@@ -9529,19 +9541,19 @@
       </c>
       <c r="C17" s="12">
         <f t="shared" si="0"/>
-        <v>0.12047752063904139</v>
+        <v>0.32673970768140631</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="1"/>
-        <v>-9.5209228766729712</v>
+        <v>-15.617274911790044</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>-23.069919211451996</v>
+        <v>-18.670855887864722</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="3"/>
-        <v>-85.972975267641999</v>
+        <v>-83.307817805874876</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="4"/>
@@ -9601,11 +9613,11 @@
       </c>
       <c r="U17" s="5">
         <f t="shared" si="16"/>
-        <v>-3.7710639831892927E-2</v>
+        <v>-3.7513811510517768E-2</v>
       </c>
       <c r="V17" s="15">
         <f t="shared" si="17"/>
-        <v>-5.6453937714440858</v>
+        <v>-5.6455221170791106</v>
       </c>
       <c r="W17" s="12">
         <v>0</v>
@@ -9624,19 +9636,19 @@
       </c>
       <c r="AA17" s="5">
         <f t="shared" si="19"/>
-        <v>-6.3009268059798913</v>
+        <v>-5.7587352000009169</v>
       </c>
       <c r="AB17" s="5">
         <f t="shared" si="20"/>
-        <v>78.455915352360776</v>
+        <v>75.024592433375801</v>
       </c>
       <c r="AC17" s="5">
         <f t="shared" si="26"/>
-        <v>-6.3664599866553919</v>
+        <v>-5.8242683806764175</v>
       </c>
       <c r="AD17" s="6">
         <f t="shared" si="27"/>
-        <v>71.426570438845516</v>
+        <v>67.995247519860527</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -9649,19 +9661,19 @@
       </c>
       <c r="C18" s="12">
         <f t="shared" si="0"/>
-        <v>0.18942536373524568</v>
+        <v>0.50704052233192842</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="1"/>
-        <v>-11.922569485639087</v>
+        <v>-19.387352078449958</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>-25.062007608626232</v>
+        <v>-20.649035329461711</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="3"/>
-        <v>-86.799276497900252</v>
+        <v>-84.675287174961667</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="4"/>
@@ -9721,11 +9733,11 @@
       </c>
       <c r="U18" s="5">
         <f t="shared" si="16"/>
-        <v>-5.9617586816831256E-2</v>
+        <v>-5.930729708284245E-2</v>
       </c>
       <c r="V18" s="15">
         <f t="shared" si="17"/>
-        <v>-7.0958875225881455</v>
+        <v>-7.0961423206272976</v>
       </c>
       <c r="W18" s="12">
         <v>0</v>
@@ -9744,19 +9756,19 @@
       </c>
       <c r="AA18" s="5">
         <f t="shared" si="19"/>
-        <v>-8.2378833844097823</v>
+        <v>-7.5703163898866395</v>
       </c>
       <c r="AB18" s="5">
         <f t="shared" si="20"/>
-        <v>76.82789278988129</v>
+        <v>71.48684472196986</v>
       </c>
       <c r="AC18" s="5">
         <f t="shared" si="26"/>
-        <v>-8.3412930852878446</v>
+        <v>-7.6737260907647027</v>
       </c>
       <c r="AD18" s="6">
         <f t="shared" si="27"/>
-        <v>68.004227403844425</v>
+        <v>62.663179335932995</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -9769,19 +9781,19 @@
       </c>
       <c r="C19" s="12">
         <f t="shared" si="0"/>
-        <v>0.29650645729707098</v>
+        <v>0.77829718381231361</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="1"/>
-        <v>-14.885859133098752</v>
+        <v>-23.894553243486335</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="2"/>
-        <v>-27.05700829872919</v>
+        <v>-22.635210862816855</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="3"/>
-        <v>-87.45659887516895</v>
+        <v>-85.765935795623719</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" si="4"/>
@@ -9841,11 +9853,11 @@
       </c>
       <c r="U19" s="5">
         <f t="shared" si="16"/>
-        <v>-9.4114589164357193E-2</v>
+        <v>-9.3626934621061308E-2</v>
       </c>
       <c r="V19" s="15">
         <f t="shared" si="17"/>
-        <v>-8.9109356973427438</v>
+        <v>-8.9114400743140756</v>
       </c>
       <c r="W19" s="12">
         <v>0</v>
@@ -9864,19 +9876,19 @@
       </c>
       <c r="AA19" s="5">
         <f t="shared" si="19"/>
-        <v>-10.125739874203312</v>
+        <v>-9.2849947902044754</v>
       </c>
       <c r="AB19" s="5">
         <f t="shared" si="20"/>
-        <v>74.571743224939482</v>
+        <v>67.253207817125798</v>
       </c>
       <c r="AC19" s="5">
         <f t="shared" si="26"/>
-        <v>-10.288511251654851</v>
+        <v>-9.447766167656015</v>
       </c>
       <c r="AD19" s="6">
         <f t="shared" si="27"/>
-        <v>63.514108772929895</v>
+        <v>56.195573365116211</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -9889,19 +9901,19 @@
       </c>
       <c r="C20" s="12">
         <f t="shared" si="0"/>
-        <v>0.46098894415027158</v>
+        <v>1.1762561462873631</v>
       </c>
       <c r="D20" s="5">
         <f t="shared" si="1"/>
-        <v>-18.502377831370602</v>
+        <v>-29.14997164019179</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>-29.053850983791772</v>
+        <v>-24.626465517037222</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="3"/>
-        <v>-87.979214926045117</v>
+        <v>-86.634503648340328</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" si="4"/>
@@ -9961,11 +9973,11 @@
       </c>
       <c r="U20" s="5">
         <f t="shared" si="16"/>
-        <v>-0.14823748092458272</v>
+        <v>-0.14747474556627732</v>
       </c>
       <c r="V20" s="15">
         <f t="shared" si="17"/>
-        <v>-11.174333179793102</v>
+        <v>-11.175327111887563</v>
       </c>
       <c r="W20" s="12">
         <v>0</v>
@@ -9984,19 +9996,19 @@
       </c>
       <c r="AA20" s="5">
         <f t="shared" si="19"/>
-        <v>-11.944249713095703</v>
+        <v>-10.864165041817797</v>
       </c>
       <c r="AB20" s="5">
         <f t="shared" si="20"/>
-        <v>71.624968324443671</v>
+        <v>62.321091861232816</v>
       </c>
       <c r="AC20" s="5">
         <f t="shared" si="26"/>
-        <v>-12.199471899301136</v>
+        <v>-11.11938722802323</v>
       </c>
       <c r="AD20" s="6">
         <f t="shared" si="27"/>
-        <v>57.803289866702855</v>
+        <v>48.499413403491999</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -10009,19 +10021,19 @@
       </c>
       <c r="C21" s="12">
         <f t="shared" si="0"/>
-        <v>0.70955060308296547</v>
+        <v>1.7406314010328459</v>
       </c>
       <c r="D21" s="5">
         <f t="shared" si="1"/>
-        <v>-22.845139541286759</v>
+        <v>-35.074525302654862</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>-31.051857671056787</v>
+        <v>-26.620938501980305</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>-88.394587729125348</v>
+        <v>-87.325556502268526</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" si="4"/>
@@ -10081,11 +10093,11 @@
       </c>
       <c r="U21" s="5">
         <f t="shared" si="16"/>
-        <v>-0.23266819594250837</v>
+        <v>-0.23148402965705184</v>
       </c>
       <c r="V21" s="15">
         <f t="shared" si="17"/>
-        <v>-13.981776722581959</v>
+        <v>-13.983721790248376</v>
       </c>
       <c r="W21" s="12">
         <v>0</v>
@@ -10104,19 +10116,19 @@
       </c>
       <c r="AA21" s="5">
         <f t="shared" si="19"/>
-        <v>-13.663477460457312</v>
+        <v>-12.263624060117538</v>
       </c>
       <c r="AB21" s="5">
         <f t="shared" si="20"/>
-        <v>67.937856845279029</v>
+        <v>56.775557243101325</v>
       </c>
       <c r="AC21" s="5">
         <f t="shared" si="26"/>
-        <v>-14.06130847811572</v>
+        <v>-12.661455077775946</v>
       </c>
       <c r="AD21" s="6">
         <f t="shared" si="27"/>
-        <v>50.728699893184221</v>
+        <v>39.566400291006516</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -10129,19 +10141,19 @@
       </c>
       <c r="C22" s="12">
         <f t="shared" si="0"/>
-        <v>1.0764858234612535</v>
+        <v>2.5075425608615243</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="1"/>
-        <v>-27.940181584384895</v>
+        <v>-41.475126758626587</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>-33.050599504845941</v>
+        <v>-28.617447568585803</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>-88.7246525427731</v>
+        <v>-87.875044600426051</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="4"/>
@@ -10201,11 +10213,11 @@
       </c>
       <c r="U22" s="5">
         <f t="shared" si="16"/>
-        <v>-0.36323186340357799</v>
+        <v>-0.36141412210125046</v>
       </c>
       <c r="V22" s="15">
         <f t="shared" si="17"/>
-        <v>-17.435684479631966</v>
+        <v>-17.439450737281014</v>
       </c>
       <c r="W22" s="12">
         <v>0</v>
@@ -10224,19 +10236,19 @@
       </c>
       <c r="AA22" s="5">
         <f t="shared" si="19"/>
-        <v>-15.243215868652578</v>
+        <v>-13.440520186661876</v>
       </c>
       <c r="AB22" s="5">
         <f t="shared" si="20"/>
-        <v>63.497943367290475</v>
+        <v>50.808839877746784</v>
       </c>
       <c r="AC22" s="5">
         <f t="shared" si="26"/>
-        <v>-15.857891261151529</v>
+        <v>-14.055195579160827</v>
       </c>
       <c r="AD22" s="6">
         <f t="shared" si="27"/>
-        <v>42.19598899006327</v>
+        <v>29.506885500519584</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -10249,19 +10261,19 @@
       </c>
       <c r="C23" s="12">
         <f t="shared" si="0"/>
-        <v>1.6011421700036839</v>
+        <v>3.4993552155715073</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="1"/>
-        <v>-33.730937776290205</v>
+        <v>-48.056802335746056</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="2"/>
-        <v>-35.049805468049144</v>
+        <v>-30.615243493831269</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="3"/>
-        <v>-88.986893760865314</v>
+        <v>-88.311802319331122</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="4"/>
@@ -10321,11 +10333,11 @@
       </c>
       <c r="U23" s="5">
         <f t="shared" si="16"/>
-        <v>-0.56249985072644271</v>
+        <v>-0.55975643553974974</v>
       </c>
       <c r="V23" s="15">
         <f t="shared" si="17"/>
-        <v>-21.633166651034951</v>
+        <v>-21.64034508174155</v>
       </c>
       <c r="W23" s="12">
         <v>0</v>
@@ -10344,19 +10356,19 @@
       </c>
       <c r="AA23" s="5">
         <f t="shared" si="19"/>
-        <v>-16.635042676591159</v>
+        <v>-14.362854974590817</v>
       </c>
       <c r="AB23" s="5">
         <f t="shared" si="20"/>
-        <v>58.358382093083968</v>
+        <v>44.700430544455713</v>
       </c>
       <c r="AC23" s="5">
         <f t="shared" si="26"/>
-        <v>-17.572645285029381</v>
+        <v>-15.30045758302904</v>
       </c>
       <c r="AD23" s="6">
         <f t="shared" si="27"/>
-        <v>32.212700305562194</v>
+        <v>18.554748756933943</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -10369,19 +10381,19 @@
       </c>
       <c r="C24" s="12">
         <f t="shared" si="0"/>
-        <v>2.3212589454717252</v>
+        <v>4.7168972352340237</v>
       </c>
       <c r="D24" s="5">
         <f t="shared" si="1"/>
-        <v>-40.049783197857352</v>
+        <v>-54.481068989838263</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" si="2"/>
-        <v>-37.049304389992031</v>
+        <v>-32.613852240909615</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="3"/>
-        <v>-89.195230158249103</v>
+        <v>-88.658873701611341</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="4"/>
@@ -10441,11 +10453,11 @@
       </c>
       <c r="U24" s="5">
         <f t="shared" si="16"/>
-        <v>-0.86084115320757648</v>
+        <v>-0.85680137080529217</v>
       </c>
       <c r="V24" s="15">
         <f t="shared" si="17"/>
-        <v>-26.644156234065811</v>
+        <v>-26.657530199715833</v>
       </c>
       <c r="W24" s="12">
         <v>0</v>
@@ -10464,19 +10476,19 @@
       </c>
       <c r="AA24" s="5">
         <f t="shared" si="19"/>
-        <v>-17.788643982887386</v>
+        <v>-15.016844494612434</v>
       </c>
       <c r="AB24" s="5">
         <f t="shared" si="20"/>
-        <v>52.654173864630771</v>
+        <v>38.745870563637581</v>
       </c>
       <c r="AC24" s="5">
         <f t="shared" si="26"/>
-        <v>-19.193432416818641</v>
+        <v>-16.421632928543687</v>
       </c>
       <c r="AD24" s="6">
         <f t="shared" si="27"/>
-        <v>20.938676054605764</v>
+        <v>7.0303727536125749</v>
       </c>
     </row>
     <row r="25" spans="1:30">
@@ -10489,19 +10501,19 @@
       </c>
       <c r="C25" s="12">
         <f t="shared" si="0"/>
-        <v>3.2630495047203101</v>
+        <v>6.1391493680555325</v>
       </c>
       <c r="D25" s="5">
         <f t="shared" si="1"/>
-        <v>-46.620519112508077</v>
+        <v>-60.447417946511848</v>
       </c>
       <c r="E25" s="5">
         <f t="shared" si="2"/>
-        <v>-39.048988201362434</v>
+        <v>-34.612974190286046</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="3"/>
-        <v>-89.360733078129272</v>
+        <v>-88.934633714902674</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="4"/>
@@ -10561,11 +10573,11 @@
       </c>
       <c r="U25" s="5">
         <f t="shared" si="16"/>
-        <v>-1.2956347806631154</v>
+        <v>-1.2898868481827594</v>
       </c>
       <c r="V25" s="15">
         <f t="shared" si="17"/>
-        <v>-32.479495303562885</v>
+        <v>-32.503642474533635</v>
       </c>
       <c r="W25" s="12">
         <v>0</v>
@@ -10584,19 +10596,19 @@
       </c>
       <c r="AA25" s="5">
         <f t="shared" si="19"/>
-        <v>-18.662119833625564</v>
+        <v>-15.407588759705639</v>
       </c>
       <c r="AB25" s="5">
         <f t="shared" si="20"/>
-        <v>46.581695856008615</v>
+        <v>33.156749214260692</v>
       </c>
       <c r="AC25" s="5">
         <f t="shared" si="26"/>
-        <v>-20.717633028097545</v>
+        <v>-17.46310195417762</v>
       </c>
       <c r="AD25" s="6">
         <f t="shared" si="27"/>
-        <v>8.6988270762513338</v>
+        <v>-4.7261195654965888</v>
       </c>
     </row>
     <row r="26" spans="1:30">
@@ -10609,19 +10621,19 @@
       </c>
       <c r="C26" s="12">
         <f t="shared" si="0"/>
-        <v>4.4323814063587061</v>
+        <v>7.7306308326607027</v>
       </c>
       <c r="D26" s="5">
         <f t="shared" si="1"/>
-        <v>-53.107367041954589</v>
+        <v>-65.754526838224578</v>
       </c>
       <c r="E26" s="5">
         <f t="shared" si="2"/>
-        <v>-41.048788687979076</v>
+        <v>-36.612420086440991</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="3"/>
-        <v>-89.492204458403208</v>
+        <v>-89.153713487081674</v>
       </c>
       <c r="G26" s="5">
         <f t="shared" si="4"/>
@@ -10681,11 +10693,11 @@
       </c>
       <c r="U26" s="5">
         <f t="shared" si="16"/>
-        <v>-1.9070104517347022</v>
+        <v>-1.8991950916088818</v>
       </c>
       <c r="V26" s="15">
         <f t="shared" si="17"/>
-        <v>-39.056879772230012</v>
+        <v>-39.098742939903673</v>
       </c>
       <c r="W26" s="12">
         <v>0</v>
@@ -10704,19 +10716,19 @@
       </c>
       <c r="AA26" s="5">
         <f t="shared" si="19"/>
-        <v>-19.232702814377266</v>
+        <v>-15.553600159383413</v>
       </c>
       <c r="AB26" s="5">
         <f t="shared" si="20"/>
-        <v>40.327782892781066</v>
+        <v>27.977250900158946</v>
       </c>
       <c r="AC26" s="5">
         <f t="shared" si="26"/>
-        <v>-22.153728212699104</v>
+        <v>-18.474625557705252</v>
       </c>
       <c r="AD26" s="6">
         <f t="shared" si="27"/>
-        <v>-4.0771874159060104</v>
+        <v>-16.42771940852813</v>
       </c>
     </row>
     <row r="27" spans="1:30">
@@ -10729,19 +10741,19 @@
       </c>
       <c r="C27" s="12">
         <f t="shared" si="0"/>
-        <v>5.8125926528171448</v>
+        <v>9.4515851049490607</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="1"/>
-        <v>-59.194962388931458</v>
+        <v>-70.315671227464549</v>
       </c>
       <c r="E27" s="5">
         <f t="shared" si="2"/>
-        <v>-43.048662798828374</v>
+        <v>-38.612070434171216</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="3"/>
-        <v>-89.596639766420594</v>
+        <v>-89.327752686967713</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="4"/>
@@ -10801,11 +10813,11 @@
       </c>
       <c r="U27" s="5">
         <f t="shared" si="16"/>
-        <v>-2.7295039642080154</v>
+        <v>-2.7194600663678608</v>
       </c>
       <c r="V27" s="15">
         <f t="shared" si="17"/>
-        <v>-46.184328645171057</v>
+        <v>-46.253463050179441</v>
       </c>
       <c r="W27" s="12">
         <v>0</v>
@@ -10824,19 +10836,19 @@
       </c>
       <c r="AA27" s="5">
         <f t="shared" si="19"/>
-        <v>-19.503089254430524</v>
+        <v>-15.480791272773336</v>
       </c>
       <c r="AB27" s="5">
         <f t="shared" si="20"/>
-        <v>33.970105327424257</v>
+        <v>23.049149163335642</v>
       </c>
       <c r="AC27" s="5">
         <f t="shared" si="26"/>
-        <v>-23.517783084198314</v>
+        <v>-19.495485102541128</v>
       </c>
       <c r="AD27" s="6">
         <f t="shared" si="27"/>
-        <v>-16.987823622718309</v>
+        <v>-27.908779786806925</v>
       </c>
     </row>
     <row r="28" spans="1:30">
@@ -10849,19 +10861,19 @@
       </c>
       <c r="C28" s="12">
         <f t="shared" si="0"/>
-        <v>7.3704941585253589</v>
+        <v>11.265822893932169</v>
       </c>
       <c r="D28" s="5">
         <f t="shared" si="1"/>
-        <v>-64.657328523174854</v>
+        <v>-74.136674215387984</v>
       </c>
       <c r="E28" s="5">
         <f t="shared" si="2"/>
-        <v>-45.048583366266506</v>
+        <v>-40.611849804018291</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="3"/>
-        <v>-89.679597624309352</v>
+        <v>-89.466005935831973</v>
       </c>
       <c r="G28" s="5">
         <f t="shared" si="4"/>
@@ -10921,11 +10933,11 @@
       </c>
       <c r="U28" s="5">
         <f t="shared" si="16"/>
-        <v>-3.7820576003044613</v>
+        <v>-3.769972669585584</v>
       </c>
       <c r="V28" s="15">
         <f t="shared" si="17"/>
-        <v>-53.584390016687067</v>
+        <v>-53.692668227449609</v>
       </c>
       <c r="W28" s="12">
         <v>0</v>
@@ -10944,19 +10956,19 @@
       </c>
       <c r="AA28" s="5">
         <f t="shared" si="19"/>
-        <v>-19.501985070864329</v>
+        <v>-15.221168575462466</v>
       </c>
       <c r="AB28" s="5">
         <f t="shared" si="20"/>
-        <v>27.402291073767149</v>
+        <v>18.02825885926887</v>
       </c>
       <c r="AC28" s="5">
         <f t="shared" si="26"/>
-        <v>-24.82910957535637</v>
+        <v>-20.548293079954504</v>
       </c>
       <c r="AD28" s="6">
         <f t="shared" si="27"/>
-        <v>-29.80804922765746</v>
+        <v>-39.182081442155734</v>
       </c>
     </row>
     <row r="29" spans="1:30">
@@ -10969,19 +10981,19 @@
       </c>
       <c r="C29" s="12">
         <f t="shared" si="0"/>
-        <v>9.0664584705723019</v>
+        <v>13.144390073469328</v>
       </c>
       <c r="D29" s="5">
         <f t="shared" si="1"/>
-        <v>-69.38363710439107</v>
+        <v>-77.28031623658849</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="2"/>
-        <v>-47.048533246960673</v>
+        <v>-42.611710590035571</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="3"/>
-        <v>-89.745494367482763</v>
+        <v>-89.575828905340558</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="4"/>
@@ -11041,11 +11053,11 @@
       </c>
       <c r="U29" s="5">
         <f t="shared" si="16"/>
-        <v>-5.0618418530133553</v>
+        <v>-5.048342683998424</v>
       </c>
       <c r="V29" s="15">
         <f t="shared" si="17"/>
-        <v>-60.962626285703365</v>
+        <v>-61.123555047521492</v>
       </c>
       <c r="W29" s="12">
         <v>0</v>
@@ -11064,19 +11076,19 @@
       </c>
       <c r="AA29" s="5">
         <f t="shared" si="19"/>
-        <v>-19.281658402839614</v>
+        <v>-14.816735706974594</v>
       </c>
       <c r="AB29" s="5">
         <f t="shared" si="20"/>
-        <v>20.330986496241863</v>
+        <v>12.443044064368522</v>
       </c>
       <c r="AC29" s="5">
         <f t="shared" si="26"/>
-        <v>-26.111291514630874</v>
+        <v>-21.646368818765854</v>
       </c>
       <c r="AD29" s="6">
         <f t="shared" si="27"/>
-        <v>-42.569881100255273</v>
+        <v>-50.457823532128614</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -11089,19 +11101,19 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="0"/>
-        <v>10.863061160118869</v>
+        <v>15.065986446381011</v>
       </c>
       <c r="D30" s="5">
         <f t="shared" si="1"/>
-        <v>-73.362419511030012</v>
+        <v>-79.835080935786934</v>
       </c>
       <c r="E30" s="5">
         <f t="shared" si="2"/>
-        <v>-49.048501623518952</v>
+        <v>-44.611622749654543</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="3"/>
-        <v>-89.79783849951059</v>
+        <v>-89.663066651548121</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="4"/>
@@ -11161,11 +11173,11 @@
       </c>
       <c r="U30" s="5">
         <f t="shared" si="16"/>
-        <v>-6.546279413588576</v>
+        <v>-6.532448736641367</v>
       </c>
       <c r="V30" s="15">
         <f t="shared" si="17"/>
-        <v>-68.089793838664022</v>
+        <v>-68.317936795441867</v>
       </c>
       <c r="W30" s="12">
         <v>0</v>
@@ -11184,19 +11196,19 @@
       </c>
       <c r="AA30" s="5">
         <f t="shared" si="19"/>
-        <v>-18.914223005295629</v>
+        <v>-14.323918901193915</v>
       </c>
       <c r="AB30" s="5">
         <f t="shared" si="20"/>
-        <v>12.35214166976283</v>
+        <v>5.7861091361905324</v>
       </c>
       <c r="AC30" s="5">
         <f t="shared" si="26"/>
-        <v>-27.397850629390796</v>
+        <v>-22.807546525289084</v>
       </c>
       <c r="AD30" s="6">
         <f t="shared" si="27"/>
-        <v>-55.527929862906134</v>
+        <v>-62.093962396478432</v>
       </c>
     </row>
     <row r="31" spans="1:30">
@@ -11209,19 +11221,19 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="0"/>
-        <v>12.7296449826101</v>
+        <v>17.015778761159147</v>
       </c>
       <c r="D31" s="5">
         <f t="shared" si="1"/>
-        <v>-76.646998095117851</v>
+        <v>-81.894435209755841</v>
       </c>
       <c r="E31" s="5">
         <f t="shared" si="2"/>
-        <v>-51.048481670357653</v>
+        <v>-46.611567325206821</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="3"/>
-        <v>-89.839417166260432</v>
+        <v>-89.732363189580028</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" si="4"/>
@@ -11281,11 +11293,11 @@
       </c>
       <c r="U31" s="5">
         <f t="shared" si="16"/>
-        <v>-8.2021326686791021</v>
+        <v>-8.1895145581431024</v>
       </c>
       <c r="V31" s="15">
         <f t="shared" si="17"/>
-        <v>-74.854892351730683</v>
+        <v>-75.165750384991298</v>
       </c>
       <c r="W31" s="12">
         <v>0</v>
@@ -11304,19 +11316,19 @@
       </c>
       <c r="AA31" s="5">
         <f t="shared" si="19"/>
-        <v>-18.483992334825494</v>
+        <v>-13.811656833561665</v>
       </c>
       <c r="AB31" s="5">
         <f t="shared" si="20"/>
-        <v>3.0655178065483435</v>
+        <v>-2.3857233646698708</v>
       </c>
       <c r="AC31" s="5">
         <f t="shared" si="26"/>
-        <v>-28.734211676491931</v>
+        <v>-24.0618761752281</v>
       </c>
       <c r="AD31" s="6">
         <f t="shared" si="27"/>
-        <v>-69.041023330989319</v>
+        <v>-74.492264502207533</v>
       </c>
     </row>
     <row r="32" spans="1:30">
@@ -11329,19 +11341,19 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" si="0"/>
-        <v>14.643306150545678</v>
+        <v>18.983798571862028</v>
       </c>
       <c r="D32" s="5">
         <f t="shared" si="1"/>
-        <v>-79.322389570050987</v>
+        <v>-83.545663292607856</v>
       </c>
       <c r="E32" s="5">
         <f t="shared" si="2"/>
-        <v>-53.048469080716814</v>
+        <v>-48.611532354380522</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" si="3"/>
-        <v>-89.872444397892806</v>
+        <v>-89.787407954210821</v>
       </c>
       <c r="G32" s="5">
         <f t="shared" si="4"/>
@@ -11401,11 +11413,11 @@
       </c>
       <c r="U32" s="5">
         <f t="shared" si="16"/>
-        <v>-9.996279435669102</v>
+        <v>-9.9869594082256725</v>
       </c>
       <c r="V32" s="15">
         <f t="shared" si="17"/>
-        <v>-81.270944574141282</v>
+        <v>-81.681133653077751</v>
       </c>
       <c r="W32" s="12">
         <v>0</v>
@@ -11424,19 +11436,19 @@
       </c>
       <c r="AA32" s="5">
         <f t="shared" si="19"/>
-        <v>-18.073984419378935</v>
+        <v>-13.350565977254906</v>
       </c>
       <c r="AB32" s="5">
         <f t="shared" si="20"/>
-        <v>-7.8449587574995352</v>
+        <v>-12.393385115310901</v>
       </c>
       <c r="AC32" s="5">
         <f t="shared" si="26"/>
-        <v>-30.170205396250175</v>
+        <v>-25.446786954126146</v>
       </c>
       <c r="AD32" s="6">
         <f t="shared" si="27"/>
-        <v>-83.46084216117076</v>
+        <v>-88.009268518982125</v>
       </c>
     </row>
     <row r="33" spans="1:30">
@@ -11449,19 +11461,19 @@
       </c>
       <c r="C33" s="12">
         <f t="shared" si="0"/>
-        <v>16.587933417723459</v>
+        <v>20.963498591188351</v>
       </c>
       <c r="D33" s="5">
         <f t="shared" si="1"/>
-        <v>-81.482211492231386</v>
+        <v>-84.865132754444772</v>
       </c>
       <c r="E33" s="5">
         <f t="shared" si="2"/>
-        <v>-55.048461137171685</v>
+        <v>-50.611510289135929</v>
       </c>
       <c r="F33" s="5">
         <f t="shared" si="3"/>
-        <v>-89.898678921974565</v>
+        <v>-89.831131849561615</v>
       </c>
       <c r="G33" s="5">
         <f t="shared" si="4"/>
@@ -11521,11 +11533,11 @@
       </c>
       <c r="U33" s="5">
         <f t="shared" si="16"/>
-        <v>-11.903711237206092</v>
+        <v>-11.900515917280197</v>
       </c>
       <c r="V33" s="15">
         <f t="shared" si="17"/>
-        <v>-87.446748116449356</v>
+        <v>-87.9739016174574</v>
       </c>
       <c r="W33" s="12">
         <v>0</v>
@@ -11544,19 +11556,19 @@
       </c>
       <c r="AA33" s="5">
         <f t="shared" si="19"/>
-        <v>-17.751770875292515</v>
+        <v>-12.999390266838018</v>
       </c>
       <c r="AB33" s="5">
         <f t="shared" si="20"/>
-        <v>-20.618725422421946</v>
+        <v>-24.461253113230413</v>
       </c>
       <c r="AC33" s="5">
         <f t="shared" si="26"/>
-        <v>-31.747938453419621</v>
+        <v>-26.995557844965123</v>
       </c>
       <c r="AD33" s="6">
         <f t="shared" si="27"/>
-        <v>-99.104320943424469</v>
+        <v>-102.94684863423294</v>
       </c>
     </row>
     <row r="34" spans="1:30">
@@ -11569,19 +11581,19 @@
       </c>
       <c r="C34" s="12">
         <f t="shared" si="0"/>
-        <v>18.552628795272732</v>
+        <v>22.950641174139651</v>
       </c>
       <c r="D34" s="5">
         <f t="shared" si="1"/>
-        <v>-83.215677022537108</v>
+        <v>-85.91719934719552</v>
       </c>
       <c r="E34" s="5">
         <f t="shared" si="2"/>
-        <v>-57.048456125126066</v>
+        <v>-52.611496366850119</v>
       </c>
       <c r="F34" s="5">
         <f t="shared" si="3"/>
-        <v>-89.919517775991082</v>
+        <v>-89.86586311682575</v>
       </c>
       <c r="G34" s="5">
         <f t="shared" si="4"/>
@@ -11641,11 +11653,11 @@
       </c>
       <c r="U34" s="5">
         <f t="shared" si="16"/>
-        <v>-13.91173637722741</v>
+        <v>-13.918535236219626</v>
       </c>
       <c r="V34" s="15">
         <f t="shared" si="17"/>
-        <v>-93.546740461969122</v>
+        <v>-94.208405820998948</v>
       </c>
       <c r="W34" s="12">
         <v>0</v>
@@ -11664,19 +11676,19 @@
       </c>
       <c r="AA34" s="5">
         <f t="shared" si="19"/>
-        <v>-17.563583473311709</v>
+        <v>-12.798740928133096</v>
       </c>
       <c r="AB34" s="5">
         <f t="shared" si="20"/>
-        <v>-35.500796591905754</v>
+        <v>-38.810329616428675</v>
       </c>
       <c r="AC34" s="5">
         <f t="shared" si="26"/>
-        <v>-33.495414619638382</v>
+        <v>-28.730572074459772</v>
       </c>
       <c r="AD34" s="6">
         <f t="shared" si="27"/>
-        <v>-116.30910318214974</v>
+        <v>-119.61863620667266</v>
       </c>
     </row>
     <row r="35" spans="1:30">
@@ -11689,19 +11701,19 @@
       </c>
       <c r="C35" s="12">
         <f t="shared" si="0"/>
-        <v>20.530204503759162</v>
+        <v>24.942509063051492</v>
       </c>
       <c r="D35" s="5">
         <f t="shared" si="1"/>
-        <v>-84.601723388558227</v>
+        <v>-86.754890201745269</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" si="2"/>
-        <v>-59.048452962736107</v>
+        <v>-54.611487582458679</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" si="3"/>
-        <v>-89.936070681559244</v>
+        <v>-89.8934512145387</v>
       </c>
       <c r="G35" s="5">
         <f t="shared" si="4"/>
@@ -11761,11 +11773,11 @@
       </c>
       <c r="U35" s="5">
         <f t="shared" si="16"/>
-        <v>-16.021492851863002</v>
+        <v>-16.0435130279233</v>
       </c>
       <c r="V35" s="15">
         <f t="shared" si="17"/>
-        <v>-99.751361396451628</v>
+        <v>-100.56214792881879</v>
       </c>
       <c r="W35" s="12">
         <v>0</v>
@@ -11784,19 +11796,19 @@
       </c>
       <c r="AA35" s="5">
         <f t="shared" si="19"/>
-        <v>-17.539930480793913</v>
+        <v>-12.77601145025651</v>
       </c>
       <c r="AB35" s="5">
         <f t="shared" si="20"/>
-        <v>-52.833729264801057</v>
+        <v>-55.755063143334745</v>
       </c>
       <c r="AC35" s="5">
         <f t="shared" si="26"/>
-        <v>-35.430672149749014</v>
+        <v>-30.666753119211613</v>
       </c>
       <c r="AD35" s="6">
         <f t="shared" si="27"/>
-        <v>-135.50938020374556</v>
+        <v>-138.43071408227925</v>
       </c>
     </row>
     <row r="36" spans="1:30">
@@ -11809,19 +11821,19 @@
       </c>
       <c r="C36" s="12">
         <f t="shared" si="0"/>
-        <v>22.515995924217091</v>
+        <v>26.937370201830419</v>
       </c>
       <c r="D36" s="5">
         <f t="shared" si="1"/>
-        <v>-85.707313113641931</v>
+        <v>-87.421300411860287</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="2"/>
-        <v>-61.048450967401742</v>
+        <v>-56.611482039873231</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" si="3"/>
-        <v>-89.949219129558855</v>
+        <v>-89.915365255328112</v>
       </c>
       <c r="G36" s="5">
         <f t="shared" si="4"/>
@@ -11881,11 +11893,11 @@
       </c>
       <c r="U36" s="5">
         <f t="shared" si="16"/>
-        <v>-18.24783000299038</v>
+        <v>-18.291792456966778</v>
       </c>
       <c r="V36" s="15">
         <f t="shared" si="17"/>
-        <v>-106.21877547003409</v>
+        <v>-107.18523082636604</v>
       </c>
       <c r="W36" s="12">
         <v>0</v>
@@ -11904,19 +11916,19 @@
       </c>
       <c r="AA36" s="5">
         <f t="shared" si="19"/>
-        <v>-17.707676995937199</v>
+        <v>-12.956626977743801</v>
       </c>
       <c r="AB36" s="5">
         <f t="shared" si="20"/>
-        <v>-73.105130303780896</v>
+        <v>-75.751719084100458</v>
       </c>
       <c r="AC36" s="5">
         <f t="shared" si="26"/>
-        <v>-37.572291492263162</v>
+        <v>-32.821241474069758</v>
       </c>
       <c r="AD36" s="6">
         <f t="shared" si="27"/>
-        <v>-157.27549358081262</v>
+        <v>-159.92208236113217</v>
       </c>
     </row>
     <row r="37" spans="1:30">
@@ -11929,19 +11941,19 @@
       </c>
       <c r="C37" s="12">
         <f t="shared" si="0"/>
-        <v>24.507006939184926</v>
+        <v>28.934124668120177</v>
       </c>
       <c r="D37" s="5">
         <f t="shared" si="1"/>
-        <v>-86.587842827738385</v>
+        <v>-87.951155684255596</v>
       </c>
       <c r="E37" s="5">
         <f t="shared" si="2"/>
-        <v>-63.048449708430418</v>
+        <v>-58.611478542734616</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="3"/>
-        <v>-89.959663316927006</v>
+        <v>-89.932772214623469</v>
       </c>
       <c r="G37" s="5">
         <f t="shared" si="4"/>
@@ -12001,11 +12013,11 @@
       </c>
       <c r="U37" s="5">
         <f t="shared" si="16"/>
-        <v>-20.617452190153003</v>
+        <v>-20.691217130661435</v>
       </c>
       <c r="V37" s="15">
         <f t="shared" si="17"/>
-        <v>-113.04485941242365</v>
+        <v>-114.15847731447803</v>
       </c>
       <c r="W37" s="12">
         <v>0</v>
@@ -12024,19 +12036,19 @@
       </c>
       <c r="AA37" s="5">
         <f t="shared" si="19"/>
-        <v>-18.100935891077082</v>
+        <v>-13.373942669926505</v>
       </c>
       <c r="AB37" s="5">
         <f t="shared" si="20"/>
-        <v>-96.942247232560518</v>
+        <v>-99.392286888828565</v>
       </c>
       <c r="AC37" s="5">
         <f t="shared" si="26"/>
-        <v>-39.948984012561297</v>
+        <v>-35.221990791410718</v>
       </c>
       <c r="AD37" s="6">
         <f t="shared" si="27"/>
-        <v>-182.30570384895836</v>
+        <v>-184.75574350522641</v>
       </c>
     </row>
     <row r="38" spans="1:30">
@@ -12049,19 +12061,19 @@
       </c>
       <c r="C38" s="12">
         <f t="shared" si="0"/>
-        <v>26.501325685061357</v>
+        <v>30.932075626125688</v>
       </c>
       <c r="D38" s="5">
         <f t="shared" si="1"/>
-        <v>-87.288444638261723</v>
+        <v>-88.372289106240288</v>
       </c>
       <c r="E38" s="5">
         <f t="shared" si="2"/>
-        <v>-65.048448914073006</v>
+        <v>-60.611476336187849</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" si="3"/>
-        <v>-89.967959431786511</v>
+        <v>-89.946599062873531</v>
       </c>
       <c r="G38" s="5">
         <f t="shared" si="4"/>
@@ -12121,11 +12133,11 @@
       </c>
       <c r="U38" s="5">
         <f t="shared" si="16"/>
-        <v>-23.164147767082927</v>
+        <v>-23.275555082264017</v>
       </c>
       <c r="V38" s="15">
         <f t="shared" si="17"/>
-        <v>-120.22379820491039</v>
+        <v>-121.45460698437938</v>
       </c>
       <c r="W38" s="12">
         <v>0</v>
@@ -12144,19 +12156,19 @@
       </c>
       <c r="AA38" s="5">
         <f t="shared" si="19"/>
-        <v>-18.76583039819457</v>
+        <v>-14.072845927398225</v>
       </c>
       <c r="AB38" s="5">
         <f t="shared" si="20"/>
-        <v>-125.0782836030878</v>
+        <v>-127.37157648162237</v>
       </c>
       <c r="AC38" s="5">
         <f t="shared" si="26"/>
-        <v>-42.603393235039213</v>
+        <v>-37.910408764242867</v>
       </c>
       <c r="AD38" s="6">
         <f t="shared" si="27"/>
-        <v>-211.39237903675581</v>
+        <v>-213.68567191529041</v>
       </c>
     </row>
     <row r="39" spans="1:30">
@@ -12169,19 +12181,19 @@
       </c>
       <c r="C39" s="12">
         <f t="shared" si="0"/>
-        <v>28.49773722828084</v>
+        <v>32.93078227042534</v>
       </c>
       <c r="D39" s="5">
         <f t="shared" si="1"/>
-        <v>-87.845541563257143</v>
+        <v>-88.706934913310263</v>
       </c>
       <c r="E39" s="5">
         <f t="shared" si="2"/>
-        <v>-67.048448412867288</v>
+        <v>-62.611474943950391</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" si="3"/>
-        <v>-89.974549271032359</v>
+        <v>-89.957582123347009</v>
       </c>
       <c r="G39" s="5">
         <f t="shared" si="4"/>
@@ -12241,11 +12253,11 @@
       </c>
       <c r="U39" s="5">
         <f t="shared" si="16"/>
-        <v>-25.920181659685131</v>
+        <v>-26.07512830542321</v>
       </c>
       <c r="V39" s="15">
         <f t="shared" si="17"/>
-        <v>-127.6237783125878</v>
+        <v>-128.91920795120214</v>
       </c>
       <c r="W39" s="12">
         <v>0</v>
@@ -12264,19 +12276,19 @@
       </c>
       <c r="AA39" s="5">
         <f t="shared" si="19"/>
-        <v>-19.758004932920791</v>
+        <v>-15.10626380056952</v>
       </c>
       <c r="AB39" s="5">
         <f t="shared" si="20"/>
-        <v>-157.58733095917952</v>
+        <v>-159.72718680016166</v>
       </c>
       <c r="AC39" s="5">
         <f t="shared" si="26"/>
-        <v>-45.588938953326902</v>
+        <v>-40.937197820975626</v>
       </c>
       <c r="AD39" s="6">
         <f t="shared" si="27"/>
-        <v>-244.65802222475335</v>
+        <v>-246.79787806573549</v>
       </c>
     </row>
     <row r="40" spans="1:30">
@@ -12289,19 +12301,19 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" si="0"/>
-        <v>30.495471538558046</v>
+        <v>34.929966019920656</v>
       </c>
       <c r="D40" s="5">
         <f t="shared" si="1"/>
-        <v>-88.288355161460544</v>
+        <v>-88.972817538247725</v>
       </c>
       <c r="E40" s="5">
         <f t="shared" si="2"/>
-        <v>-69.048448096627851</v>
+        <v>-64.611474065507721</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" si="3"/>
-        <v>-89.979783766895991</v>
+        <v>-89.966306280645753</v>
       </c>
       <c r="G40" s="5">
         <f t="shared" si="4"/>
@@ -12361,11 +12373,11 @@
       </c>
       <c r="U40" s="5">
         <f t="shared" si="16"/>
-        <v>-28.905410038664868</v>
+        <v>-29.105924807113777</v>
       </c>
       <c r="V40" s="15">
         <f t="shared" si="17"/>
-        <v>-135.00017184055085</v>
+        <v>-136.29321329632947</v>
       </c>
       <c r="W40" s="12">
         <v>0</v>
@@ -12384,19 +12396,19 @@
       </c>
       <c r="AA40" s="5">
         <f t="shared" si="19"/>
-        <v>-21.135187358487823</v>
+        <v>-16.527564347426022</v>
       </c>
       <c r="AB40" s="5">
         <f t="shared" si="20"/>
-        <v>-173.35104567206403</v>
+        <v>-175.3150720183796</v>
       </c>
       <c r="AC40" s="5">
         <f t="shared" si="26"/>
-        <v>-48.961933666525013</v>
+        <v>-44.354310655463209</v>
       </c>
       <c r="AD40" s="6">
         <f t="shared" si="27"/>
-        <v>-261.0234648153745</v>
+        <v>-262.98749116169006</v>
       </c>
     </row>
     <row r="41" spans="1:30">
@@ -12409,19 +12421,19 @@
       </c>
       <c r="C41" s="12">
         <f t="shared" si="0"/>
-        <v>32.494041376571957</v>
+        <v>36.929450921722577</v>
       </c>
       <c r="D41" s="5">
         <f t="shared" si="1"/>
-        <v>-88.64024291147409</v>
+        <v>-89.184047709050915</v>
       </c>
       <c r="E41" s="5">
         <f t="shared" si="2"/>
-        <v>-71.048447897094206</v>
+        <v>-66.611473511247766</v>
       </c>
       <c r="F41" s="5">
         <f t="shared" si="3"/>
-        <v>-89.983941674999798</v>
+        <v>-89.973236126245482</v>
       </c>
       <c r="G41" s="5">
         <f t="shared" si="4"/>
@@ -12481,11 +12493,11 @@
       </c>
       <c r="U41" s="5">
         <f t="shared" si="16"/>
-        <v>-32.119026630650765</v>
+        <v>-32.362522856470434</v>
       </c>
       <c r="V41" s="15">
         <f t="shared" si="17"/>
-        <v>-142.05551248526746</v>
+        <v>-143.28040486604999</v>
       </c>
       <c r="W41" s="12">
         <v>0</v>
@@ -12504,19 +12516,19 @@
       </c>
       <c r="AA41" s="5">
         <f t="shared" si="19"/>
-        <v>-22.949531860442413</v>
+        <v>-18.383974888237063</v>
       </c>
       <c r="AB41" s="5">
         <f t="shared" si="20"/>
-        <v>-190.08918701832195</v>
+        <v>-191.847178647927</v>
       </c>
       <c r="AC41" s="5">
         <f t="shared" si="26"/>
-        <v>-52.773633821396245</v>
+        <v>-48.208076849190903</v>
       </c>
       <c r="AD41" s="6">
         <f t="shared" si="27"/>
-        <v>-278.23994847241528</v>
+        <v>-279.99794010202032</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -12529,19 +12541,19 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" si="0"/>
-        <v>34.493138762977573</v>
+        <v>38.929125885293928</v>
       </c>
       <c r="D42" s="5">
         <f t="shared" si="1"/>
-        <v>-88.919831718162442</v>
+        <v>-89.351849887252214</v>
       </c>
       <c r="E42" s="5">
         <f t="shared" si="2"/>
-        <v>-73.048447771197004</v>
+        <v>-68.61147316153334</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" si="3"/>
-        <v>-89.987244418926707</v>
+        <v>-89.978740698835551</v>
       </c>
       <c r="G42" s="5">
         <f t="shared" si="4"/>
@@ -12601,11 +12613,11 @@
       </c>
       <c r="U42" s="5">
         <f t="shared" si="16"/>
-        <v>-35.538961034859248</v>
+        <v>-35.819206827509241</v>
       </c>
       <c r="V42" s="15">
         <f t="shared" si="17"/>
-        <v>-148.52254214603312</v>
+        <v>-149.62983109828511</v>
       </c>
       <c r="W42" s="12">
         <v>0</v>
@@ -12624,22 +12636,22 @@
       </c>
       <c r="AA42" s="5">
         <f t="shared" si="19"/>
-        <v>-25.243363600862985</v>
+        <v>-20.713978394505006</v>
       </c>
       <c r="AB42" s="5">
         <f t="shared" si="20"/>
-        <v>-207.50827623306952</v>
+        <v>-209.03907963432016</v>
       </c>
       <c r="AC42" s="5">
         <f t="shared" si="26"/>
-        <v>-57.065796262774811</v>
+        <v>-52.536411056416839</v>
       </c>
       <c r="AD42" s="6">
         <f t="shared" si="27"/>
-        <v>-296.03918560911262</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30" ht="13.8" thickBot="1">
+        <v>-297.56998901036326</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" ht="13" thickBot="1">
       <c r="A43" s="7">
         <v>5</v>
       </c>
@@ -12649,19 +12661,19 @@
       </c>
       <c r="C43" s="13">
         <f t="shared" si="0"/>
-        <v>36.492569155762553</v>
+        <v>40.928920788654565</v>
       </c>
       <c r="D43" s="8">
         <f t="shared" si="1"/>
-        <v>-89.141954321980336</v>
+        <v>-89.485147960384239</v>
       </c>
       <c r="E43" s="8">
         <f t="shared" si="2"/>
-        <v>-75.04844769176124</v>
+        <v>-70.611472940878443</v>
       </c>
       <c r="F43" s="8">
         <f t="shared" si="3"/>
-        <v>-89.98986788174139</v>
+        <v>-89.983113136548582</v>
       </c>
       <c r="G43" s="8">
         <f t="shared" si="4"/>
@@ -12721,11 +12733,11 @@
       </c>
       <c r="U43" s="8">
         <f t="shared" si="16"/>
-        <v>-39.129075746036037</v>
+        <v>-39.438196880887865</v>
       </c>
       <c r="V43" s="16">
         <f t="shared" si="17"/>
-        <v>-154.2267387674656</v>
+        <v>-155.19012216650759</v>
       </c>
       <c r="W43" s="13">
         <v>0</v>
@@ -12744,22 +12756,22 @@
       </c>
       <c r="AA43" s="8">
         <f t="shared" si="19"/>
-        <v>-28.047163224972959</v>
+        <v>-23.546288709022019</v>
       </c>
       <c r="AB43" s="8">
         <f t="shared" si="20"/>
-        <v>-225.23889578881941</v>
+        <v>-226.53871808107249</v>
       </c>
       <c r="AC43" s="8">
         <f t="shared" si="26"/>
-        <v>-61.868542300159561</v>
+        <v>-57.367667784208621</v>
       </c>
       <c r="AD43" s="17">
         <f t="shared" si="27"/>
-        <v>-314.07186125076487</v>
-      </c>
-    </row>
-    <row r="44" spans="1:30" ht="13.8" thickTop="1"/>
+        <v>-315.37168354301792</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" ht="13" thickTop="1"/>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{0F8159A6-236F-4F54-A569-A835A6AD5DA8}" scale="70" state="hidden" topLeftCell="D1">
@@ -12791,139 +12803,139 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="128" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
     <col min="257" max="257" width="128" customWidth="1"/>
-    <col min="258" max="258" width="13.6640625" customWidth="1"/>
+    <col min="258" max="258" width="13.6328125" customWidth="1"/>
     <col min="513" max="513" width="128" customWidth="1"/>
-    <col min="514" max="514" width="13.6640625" customWidth="1"/>
+    <col min="514" max="514" width="13.6328125" customWidth="1"/>
     <col min="769" max="769" width="128" customWidth="1"/>
-    <col min="770" max="770" width="13.6640625" customWidth="1"/>
+    <col min="770" max="770" width="13.6328125" customWidth="1"/>
     <col min="1025" max="1025" width="128" customWidth="1"/>
-    <col min="1026" max="1026" width="13.6640625" customWidth="1"/>
+    <col min="1026" max="1026" width="13.6328125" customWidth="1"/>
     <col min="1281" max="1281" width="128" customWidth="1"/>
-    <col min="1282" max="1282" width="13.6640625" customWidth="1"/>
+    <col min="1282" max="1282" width="13.6328125" customWidth="1"/>
     <col min="1537" max="1537" width="128" customWidth="1"/>
-    <col min="1538" max="1538" width="13.6640625" customWidth="1"/>
+    <col min="1538" max="1538" width="13.6328125" customWidth="1"/>
     <col min="1793" max="1793" width="128" customWidth="1"/>
-    <col min="1794" max="1794" width="13.6640625" customWidth="1"/>
+    <col min="1794" max="1794" width="13.6328125" customWidth="1"/>
     <col min="2049" max="2049" width="128" customWidth="1"/>
-    <col min="2050" max="2050" width="13.6640625" customWidth="1"/>
+    <col min="2050" max="2050" width="13.6328125" customWidth="1"/>
     <col min="2305" max="2305" width="128" customWidth="1"/>
-    <col min="2306" max="2306" width="13.6640625" customWidth="1"/>
+    <col min="2306" max="2306" width="13.6328125" customWidth="1"/>
     <col min="2561" max="2561" width="128" customWidth="1"/>
-    <col min="2562" max="2562" width="13.6640625" customWidth="1"/>
+    <col min="2562" max="2562" width="13.6328125" customWidth="1"/>
     <col min="2817" max="2817" width="128" customWidth="1"/>
-    <col min="2818" max="2818" width="13.6640625" customWidth="1"/>
+    <col min="2818" max="2818" width="13.6328125" customWidth="1"/>
     <col min="3073" max="3073" width="128" customWidth="1"/>
-    <col min="3074" max="3074" width="13.6640625" customWidth="1"/>
+    <col min="3074" max="3074" width="13.6328125" customWidth="1"/>
     <col min="3329" max="3329" width="128" customWidth="1"/>
-    <col min="3330" max="3330" width="13.6640625" customWidth="1"/>
+    <col min="3330" max="3330" width="13.6328125" customWidth="1"/>
     <col min="3585" max="3585" width="128" customWidth="1"/>
-    <col min="3586" max="3586" width="13.6640625" customWidth="1"/>
+    <col min="3586" max="3586" width="13.6328125" customWidth="1"/>
     <col min="3841" max="3841" width="128" customWidth="1"/>
-    <col min="3842" max="3842" width="13.6640625" customWidth="1"/>
+    <col min="3842" max="3842" width="13.6328125" customWidth="1"/>
     <col min="4097" max="4097" width="128" customWidth="1"/>
-    <col min="4098" max="4098" width="13.6640625" customWidth="1"/>
+    <col min="4098" max="4098" width="13.6328125" customWidth="1"/>
     <col min="4353" max="4353" width="128" customWidth="1"/>
-    <col min="4354" max="4354" width="13.6640625" customWidth="1"/>
+    <col min="4354" max="4354" width="13.6328125" customWidth="1"/>
     <col min="4609" max="4609" width="128" customWidth="1"/>
-    <col min="4610" max="4610" width="13.6640625" customWidth="1"/>
+    <col min="4610" max="4610" width="13.6328125" customWidth="1"/>
     <col min="4865" max="4865" width="128" customWidth="1"/>
-    <col min="4866" max="4866" width="13.6640625" customWidth="1"/>
+    <col min="4866" max="4866" width="13.6328125" customWidth="1"/>
     <col min="5121" max="5121" width="128" customWidth="1"/>
-    <col min="5122" max="5122" width="13.6640625" customWidth="1"/>
+    <col min="5122" max="5122" width="13.6328125" customWidth="1"/>
     <col min="5377" max="5377" width="128" customWidth="1"/>
-    <col min="5378" max="5378" width="13.6640625" customWidth="1"/>
+    <col min="5378" max="5378" width="13.6328125" customWidth="1"/>
     <col min="5633" max="5633" width="128" customWidth="1"/>
-    <col min="5634" max="5634" width="13.6640625" customWidth="1"/>
+    <col min="5634" max="5634" width="13.6328125" customWidth="1"/>
     <col min="5889" max="5889" width="128" customWidth="1"/>
-    <col min="5890" max="5890" width="13.6640625" customWidth="1"/>
+    <col min="5890" max="5890" width="13.6328125" customWidth="1"/>
     <col min="6145" max="6145" width="128" customWidth="1"/>
-    <col min="6146" max="6146" width="13.6640625" customWidth="1"/>
+    <col min="6146" max="6146" width="13.6328125" customWidth="1"/>
     <col min="6401" max="6401" width="128" customWidth="1"/>
-    <col min="6402" max="6402" width="13.6640625" customWidth="1"/>
+    <col min="6402" max="6402" width="13.6328125" customWidth="1"/>
     <col min="6657" max="6657" width="128" customWidth="1"/>
-    <col min="6658" max="6658" width="13.6640625" customWidth="1"/>
+    <col min="6658" max="6658" width="13.6328125" customWidth="1"/>
     <col min="6913" max="6913" width="128" customWidth="1"/>
-    <col min="6914" max="6914" width="13.6640625" customWidth="1"/>
+    <col min="6914" max="6914" width="13.6328125" customWidth="1"/>
     <col min="7169" max="7169" width="128" customWidth="1"/>
-    <col min="7170" max="7170" width="13.6640625" customWidth="1"/>
+    <col min="7170" max="7170" width="13.6328125" customWidth="1"/>
     <col min="7425" max="7425" width="128" customWidth="1"/>
-    <col min="7426" max="7426" width="13.6640625" customWidth="1"/>
+    <col min="7426" max="7426" width="13.6328125" customWidth="1"/>
     <col min="7681" max="7681" width="128" customWidth="1"/>
-    <col min="7682" max="7682" width="13.6640625" customWidth="1"/>
+    <col min="7682" max="7682" width="13.6328125" customWidth="1"/>
     <col min="7937" max="7937" width="128" customWidth="1"/>
-    <col min="7938" max="7938" width="13.6640625" customWidth="1"/>
+    <col min="7938" max="7938" width="13.6328125" customWidth="1"/>
     <col min="8193" max="8193" width="128" customWidth="1"/>
-    <col min="8194" max="8194" width="13.6640625" customWidth="1"/>
+    <col min="8194" max="8194" width="13.6328125" customWidth="1"/>
     <col min="8449" max="8449" width="128" customWidth="1"/>
-    <col min="8450" max="8450" width="13.6640625" customWidth="1"/>
+    <col min="8450" max="8450" width="13.6328125" customWidth="1"/>
     <col min="8705" max="8705" width="128" customWidth="1"/>
-    <col min="8706" max="8706" width="13.6640625" customWidth="1"/>
+    <col min="8706" max="8706" width="13.6328125" customWidth="1"/>
     <col min="8961" max="8961" width="128" customWidth="1"/>
-    <col min="8962" max="8962" width="13.6640625" customWidth="1"/>
+    <col min="8962" max="8962" width="13.6328125" customWidth="1"/>
     <col min="9217" max="9217" width="128" customWidth="1"/>
-    <col min="9218" max="9218" width="13.6640625" customWidth="1"/>
+    <col min="9218" max="9218" width="13.6328125" customWidth="1"/>
     <col min="9473" max="9473" width="128" customWidth="1"/>
-    <col min="9474" max="9474" width="13.6640625" customWidth="1"/>
+    <col min="9474" max="9474" width="13.6328125" customWidth="1"/>
     <col min="9729" max="9729" width="128" customWidth="1"/>
-    <col min="9730" max="9730" width="13.6640625" customWidth="1"/>
+    <col min="9730" max="9730" width="13.6328125" customWidth="1"/>
     <col min="9985" max="9985" width="128" customWidth="1"/>
-    <col min="9986" max="9986" width="13.6640625" customWidth="1"/>
+    <col min="9986" max="9986" width="13.6328125" customWidth="1"/>
     <col min="10241" max="10241" width="128" customWidth="1"/>
-    <col min="10242" max="10242" width="13.6640625" customWidth="1"/>
+    <col min="10242" max="10242" width="13.6328125" customWidth="1"/>
     <col min="10497" max="10497" width="128" customWidth="1"/>
-    <col min="10498" max="10498" width="13.6640625" customWidth="1"/>
+    <col min="10498" max="10498" width="13.6328125" customWidth="1"/>
     <col min="10753" max="10753" width="128" customWidth="1"/>
-    <col min="10754" max="10754" width="13.6640625" customWidth="1"/>
+    <col min="10754" max="10754" width="13.6328125" customWidth="1"/>
     <col min="11009" max="11009" width="128" customWidth="1"/>
-    <col min="11010" max="11010" width="13.6640625" customWidth="1"/>
+    <col min="11010" max="11010" width="13.6328125" customWidth="1"/>
     <col min="11265" max="11265" width="128" customWidth="1"/>
-    <col min="11266" max="11266" width="13.6640625" customWidth="1"/>
+    <col min="11266" max="11266" width="13.6328125" customWidth="1"/>
     <col min="11521" max="11521" width="128" customWidth="1"/>
-    <col min="11522" max="11522" width="13.6640625" customWidth="1"/>
+    <col min="11522" max="11522" width="13.6328125" customWidth="1"/>
     <col min="11777" max="11777" width="128" customWidth="1"/>
-    <col min="11778" max="11778" width="13.6640625" customWidth="1"/>
+    <col min="11778" max="11778" width="13.6328125" customWidth="1"/>
     <col min="12033" max="12033" width="128" customWidth="1"/>
-    <col min="12034" max="12034" width="13.6640625" customWidth="1"/>
+    <col min="12034" max="12034" width="13.6328125" customWidth="1"/>
     <col min="12289" max="12289" width="128" customWidth="1"/>
-    <col min="12290" max="12290" width="13.6640625" customWidth="1"/>
+    <col min="12290" max="12290" width="13.6328125" customWidth="1"/>
     <col min="12545" max="12545" width="128" customWidth="1"/>
-    <col min="12546" max="12546" width="13.6640625" customWidth="1"/>
+    <col min="12546" max="12546" width="13.6328125" customWidth="1"/>
     <col min="12801" max="12801" width="128" customWidth="1"/>
-    <col min="12802" max="12802" width="13.6640625" customWidth="1"/>
+    <col min="12802" max="12802" width="13.6328125" customWidth="1"/>
     <col min="13057" max="13057" width="128" customWidth="1"/>
-    <col min="13058" max="13058" width="13.6640625" customWidth="1"/>
+    <col min="13058" max="13058" width="13.6328125" customWidth="1"/>
     <col min="13313" max="13313" width="128" customWidth="1"/>
-    <col min="13314" max="13314" width="13.6640625" customWidth="1"/>
+    <col min="13314" max="13314" width="13.6328125" customWidth="1"/>
     <col min="13569" max="13569" width="128" customWidth="1"/>
-    <col min="13570" max="13570" width="13.6640625" customWidth="1"/>
+    <col min="13570" max="13570" width="13.6328125" customWidth="1"/>
     <col min="13825" max="13825" width="128" customWidth="1"/>
-    <col min="13826" max="13826" width="13.6640625" customWidth="1"/>
+    <col min="13826" max="13826" width="13.6328125" customWidth="1"/>
     <col min="14081" max="14081" width="128" customWidth="1"/>
-    <col min="14082" max="14082" width="13.6640625" customWidth="1"/>
+    <col min="14082" max="14082" width="13.6328125" customWidth="1"/>
     <col min="14337" max="14337" width="128" customWidth="1"/>
-    <col min="14338" max="14338" width="13.6640625" customWidth="1"/>
+    <col min="14338" max="14338" width="13.6328125" customWidth="1"/>
     <col min="14593" max="14593" width="128" customWidth="1"/>
-    <col min="14594" max="14594" width="13.6640625" customWidth="1"/>
+    <col min="14594" max="14594" width="13.6328125" customWidth="1"/>
     <col min="14849" max="14849" width="128" customWidth="1"/>
-    <col min="14850" max="14850" width="13.6640625" customWidth="1"/>
+    <col min="14850" max="14850" width="13.6328125" customWidth="1"/>
     <col min="15105" max="15105" width="128" customWidth="1"/>
-    <col min="15106" max="15106" width="13.6640625" customWidth="1"/>
+    <col min="15106" max="15106" width="13.6328125" customWidth="1"/>
     <col min="15361" max="15361" width="128" customWidth="1"/>
-    <col min="15362" max="15362" width="13.6640625" customWidth="1"/>
+    <col min="15362" max="15362" width="13.6328125" customWidth="1"/>
     <col min="15617" max="15617" width="128" customWidth="1"/>
-    <col min="15618" max="15618" width="13.6640625" customWidth="1"/>
+    <col min="15618" max="15618" width="13.6328125" customWidth="1"/>
     <col min="15873" max="15873" width="128" customWidth="1"/>
-    <col min="15874" max="15874" width="13.6640625" customWidth="1"/>
+    <col min="15874" max="15874" width="13.6328125" customWidth="1"/>
     <col min="16129" max="16129" width="128" customWidth="1"/>
-    <col min="16130" max="16130" width="13.6640625" customWidth="1"/>
+    <col min="16130" max="16130" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="66">
+    <row r="1" spans="1:1" ht="62.5">
       <c r="A1" s="25" t="s">
         <v>291</v>
       </c>
@@ -12931,7 +12943,7 @@
     <row r="2" spans="1:1">
       <c r="A2" s="9"/>
     </row>
-    <row r="3" spans="1:1" ht="79.2">
+    <row r="3" spans="1:1" ht="75">
       <c r="A3" s="25" t="s">
         <v>292</v>
       </c>
@@ -12939,7 +12951,7 @@
     <row r="4" spans="1:1">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:1" ht="52.8">
+    <row r="5" spans="1:1" ht="50">
       <c r="A5" s="25" t="s">
         <v>293</v>
       </c>
@@ -12947,7 +12959,7 @@
     <row r="6" spans="1:1">
       <c r="A6" s="9"/>
     </row>
-    <row r="7" spans="1:1" ht="79.2">
+    <row r="7" spans="1:1" ht="75">
       <c r="A7" s="25" t="s">
         <v>294</v>
       </c>

</xml_diff>